<commit_message>
i263--add and update some eit2 suites
</commit_message>
<xml_diff>
--- a/tmp_client/doc/TMP_EIT_suites/debug_10_reveal_inserter_all.xlsx
+++ b/tmp_client/doc/TMP_EIT_suites/debug_10_reveal_inserter_all.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwang1\Desktop\updates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwang1\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="0sngsN6DrFUqmuDZZhkIhd0EivD5xjZ0nj5fkMPZg+GIws2dGdQ895P+5SBGWtagLIQbEIRaHiBSjM2rhskk/Q==" workbookSaltValue="j22CHco5Hi8vlbKkcb9mlg==" workbookSpinCount="100000" lockStructure="1"/>
@@ -26,15 +26,15 @@
   </definedNames>
   <calcPr calcId="122211"/>
   <customWorkbookViews>
+    <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="2"/>
+    <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" mergeInterval="0" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
     <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
-    <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" mergeInterval="0" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
-    <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="2"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="432">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="434">
   <si>
     <t>[suite_info]</t>
   </si>
@@ -1069,9 +1069,6 @@
     <t>cmd = python DEV/bin/run_radiant.py  --run-map  --check-conf=reveal.conf</t>
   </si>
   <si>
-    <t>radiant=ng2_0</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
@@ -1553,6 +1550,15 @@
   </si>
   <si>
     <t>debug_10_reveal_inserter_all</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>HDL_syntax/02_Jedi/security_flow/12_security</t>
+  </si>
+  <si>
+    <t>radiant=ng2_1</t>
   </si>
 </sst>
 </file>
@@ -2848,46 +2854,30 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="22" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="37" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="38" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="39" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="41" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="24" xfId="41" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="21" xfId="41" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="25" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="26" xfId="41" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="41" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="22" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="35" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="44" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="44" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="44" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="21" xfId="41" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="33" xfId="41" applyBorder="1" applyAlignment="1">
@@ -2895,6 +2885,9 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="26" xfId="41" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="26" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="37" xfId="41" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2911,17 +2904,30 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="41" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="22" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="35" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="37" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="44" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="38" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="44" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="39" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="44" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="24" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="25" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="48">
@@ -5404,7 +5410,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{533732DE-155D-4F60-9C70-5866F92E7379}" diskRevisions="1" revisionId="856" version="8">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{8E4B05B1-3E12-4F85-983B-CA42D07E19EC}" diskRevisions="1" revisionId="1018" version="13">
   <header guid="{DB40D02A-1C38-451A-8E02-505A412F9BEE}" dateTime="2020-03-04T15:04:22" maxSheetId="5" userName="Jason Wang" r:id="rId1">
     <sheetIdMap count="4">
       <sheetId val="1"/>
@@ -5469,11 +5475,1253 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
+  <header guid="{FD689668-6163-46D8-A8D7-2898BB2B5407}" dateTime="2020-03-25T10:47:58" maxSheetId="5" userName="Jason Wang" r:id="rId9" minRId="857" maxRId="859">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{8C0C2131-2A5B-46ED-9C99-6C3A91A848DB}" dateTime="2020-03-25T10:48:12" maxSheetId="5" userName="Jason Wang" r:id="rId10" minRId="861" maxRId="862">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{8FB93CF3-A602-48E8-BE83-E0D933D876FA}" dateTime="2020-03-25T10:49:41" maxSheetId="5" userName="Jason Wang" r:id="rId11" minRId="864" maxRId="939">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{A7E1C060-67CC-4B0F-A2DA-C5D2A641750F}" dateTime="2020-03-25T10:53:56" maxSheetId="5" userName="Jason Wang" r:id="rId12" minRId="941">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{8E4B05B1-3E12-4F85-983B-CA42D07E19EC}" dateTime="2020-03-25T10:54:36" maxSheetId="5" userName="Jason Wang" r:id="rId13" minRId="942" maxRId="1017">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
 <file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
+</file>
+
+<file path=xl/revisions/revisionLog10.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="861" sId="2" numFmtId="30">
+    <nc r="F82">
+      <v>2</v>
+    </nc>
+  </rcc>
+  <rcc rId="862" sId="2">
+    <nc r="S82" t="inlineStr">
+      <is>
+        <t>reveal</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="delete"/>
+  <rdn rId="0" localSheetId="2" customView="1" name="Z_E811CF45_D5B3_4449_84AE_1514F9E9258F_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>case!$A$2:$AD$2</formula>
+    <oldFormula>case!$A$2:$AD$2</oldFormula>
+  </rdn>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog11.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="864" sId="2">
+    <nc r="B4" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="865" sId="2">
+    <nc r="B5" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="866" sId="2">
+    <nc r="B6" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="867" sId="2">
+    <nc r="B7" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="868" sId="2">
+    <nc r="B8" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="869" sId="2">
+    <nc r="B9" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="870" sId="2">
+    <nc r="B10" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="871" sId="2">
+    <nc r="B11" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="872" sId="2">
+    <nc r="B12" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="873" sId="2">
+    <nc r="B13" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="874" sId="2">
+    <nc r="B14" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="875" sId="2">
+    <nc r="B15" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="876" sId="2">
+    <nc r="B16" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="877" sId="2">
+    <nc r="B17" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="878" sId="2">
+    <nc r="B18" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="879" sId="2">
+    <nc r="B19" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="880" sId="2">
+    <nc r="B20" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="881" sId="2">
+    <nc r="B21" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="882" sId="2">
+    <nc r="B22" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="883" sId="2">
+    <nc r="B23" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="884" sId="2">
+    <nc r="B24" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="885" sId="2">
+    <nc r="B25" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="886" sId="2">
+    <nc r="B26" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="887" sId="2">
+    <nc r="B27" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="888" sId="2">
+    <nc r="B28" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="889" sId="2">
+    <nc r="B29" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="890" sId="2">
+    <nc r="B30" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="891" sId="2">
+    <nc r="B31" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="892" sId="2">
+    <nc r="B32" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="893" sId="2">
+    <nc r="B33" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="894" sId="2">
+    <nc r="B34" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="895" sId="2">
+    <nc r="B35" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="896" sId="2">
+    <nc r="B36" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="897" sId="2">
+    <nc r="B37" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="898" sId="2">
+    <nc r="B38" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="899" sId="2">
+    <nc r="B39" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="900" sId="2">
+    <nc r="B40" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="901" sId="2">
+    <nc r="B41" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="902" sId="2">
+    <nc r="B42" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="903" sId="2">
+    <nc r="B43" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="904" sId="2">
+    <nc r="B44" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="905" sId="2">
+    <nc r="B45" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="906" sId="2">
+    <nc r="B46" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="907" sId="2">
+    <nc r="B47" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="908" sId="2">
+    <nc r="B48" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="909" sId="2">
+    <nc r="B49" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="910" sId="2">
+    <nc r="B50" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="911" sId="2">
+    <nc r="B51" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="912" sId="2">
+    <nc r="B52" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="913" sId="2">
+    <nc r="B53" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="914" sId="2">
+    <nc r="B54" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="915" sId="2">
+    <nc r="B55" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="916" sId="2">
+    <nc r="B56" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="917" sId="2">
+    <nc r="B57" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="918" sId="2">
+    <nc r="B58" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="919" sId="2">
+    <nc r="B59" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="920" sId="2">
+    <nc r="B60" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="921" sId="2">
+    <nc r="B61" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="922" sId="2">
+    <nc r="B62" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="923" sId="2">
+    <nc r="B63" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="924" sId="2">
+    <nc r="B64" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="925" sId="2">
+    <nc r="B65" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="926" sId="2">
+    <nc r="B66" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="927" sId="2">
+    <nc r="B67" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="928" sId="2">
+    <nc r="B68" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="929" sId="2">
+    <nc r="B69" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="930" sId="2">
+    <nc r="B70" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="931" sId="2">
+    <nc r="B71" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="932" sId="2">
+    <nc r="B72" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="933" sId="2">
+    <nc r="B73" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="934" sId="2">
+    <nc r="B74" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="935" sId="2">
+    <nc r="B75" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="936" sId="2">
+    <nc r="B76" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="937" sId="2">
+    <nc r="B77" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="938" sId="2">
+    <nc r="B78" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="939" sId="2">
+    <nc r="B79" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="delete"/>
+  <rdn rId="0" localSheetId="2" customView="1" name="Z_E811CF45_D5B3_4449_84AE_1514F9E9258F_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>case!$A$2:$AD$2</formula>
+    <oldFormula>case!$A$2:$AD$2</oldFormula>
+  </rdn>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog12.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="941" sId="1">
+    <oc r="B8" t="inlineStr">
+      <is>
+        <t>radiant=ng2_0</t>
+      </is>
+    </oc>
+    <nc r="B8" t="inlineStr">
+      <is>
+        <t>radiant=ng2_1</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog13.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="942" sId="2">
+    <oc r="B4" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B4"/>
+  </rcc>
+  <rcc rId="943" sId="2">
+    <oc r="B5" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B5"/>
+  </rcc>
+  <rcc rId="944" sId="2">
+    <oc r="B6" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B6"/>
+  </rcc>
+  <rcc rId="945" sId="2">
+    <oc r="B7" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B7"/>
+  </rcc>
+  <rcc rId="946" sId="2">
+    <oc r="B8" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B8"/>
+  </rcc>
+  <rcc rId="947" sId="2">
+    <oc r="B9" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B9"/>
+  </rcc>
+  <rcc rId="948" sId="2">
+    <oc r="B10" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B10"/>
+  </rcc>
+  <rcc rId="949" sId="2">
+    <oc r="B11" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B11"/>
+  </rcc>
+  <rcc rId="950" sId="2">
+    <oc r="B12" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B12"/>
+  </rcc>
+  <rcc rId="951" sId="2">
+    <oc r="B13" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B13"/>
+  </rcc>
+  <rcc rId="952" sId="2">
+    <oc r="B14" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B14"/>
+  </rcc>
+  <rcc rId="953" sId="2">
+    <oc r="B15" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B15"/>
+  </rcc>
+  <rcc rId="954" sId="2">
+    <oc r="B16" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B16"/>
+  </rcc>
+  <rcc rId="955" sId="2">
+    <oc r="B17" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B17"/>
+  </rcc>
+  <rcc rId="956" sId="2">
+    <oc r="B18" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B18"/>
+  </rcc>
+  <rcc rId="957" sId="2">
+    <oc r="B19" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B19"/>
+  </rcc>
+  <rcc rId="958" sId="2">
+    <oc r="B20" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B20"/>
+  </rcc>
+  <rcc rId="959" sId="2">
+    <oc r="B21" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B21"/>
+  </rcc>
+  <rcc rId="960" sId="2">
+    <oc r="B22" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B22"/>
+  </rcc>
+  <rcc rId="961" sId="2">
+    <oc r="B23" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B23"/>
+  </rcc>
+  <rcc rId="962" sId="2">
+    <oc r="B24" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B24"/>
+  </rcc>
+  <rcc rId="963" sId="2">
+    <oc r="B25" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B25"/>
+  </rcc>
+  <rcc rId="964" sId="2">
+    <oc r="B26" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B26"/>
+  </rcc>
+  <rcc rId="965" sId="2">
+    <oc r="B27" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B27"/>
+  </rcc>
+  <rcc rId="966" sId="2">
+    <oc r="B28" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B28"/>
+  </rcc>
+  <rcc rId="967" sId="2">
+    <oc r="B29" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B29"/>
+  </rcc>
+  <rcc rId="968" sId="2">
+    <oc r="B30" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B30"/>
+  </rcc>
+  <rcc rId="969" sId="2">
+    <oc r="B31" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B31"/>
+  </rcc>
+  <rcc rId="970" sId="2">
+    <oc r="B32" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B32"/>
+  </rcc>
+  <rcc rId="971" sId="2">
+    <oc r="B33" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B33"/>
+  </rcc>
+  <rcc rId="972" sId="2">
+    <oc r="B34" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B34"/>
+  </rcc>
+  <rcc rId="973" sId="2">
+    <oc r="B35" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B35"/>
+  </rcc>
+  <rcc rId="974" sId="2">
+    <oc r="B36" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B36"/>
+  </rcc>
+  <rcc rId="975" sId="2">
+    <oc r="B37" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B37"/>
+  </rcc>
+  <rcc rId="976" sId="2">
+    <oc r="B38" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B38"/>
+  </rcc>
+  <rcc rId="977" sId="2">
+    <oc r="B39" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B39"/>
+  </rcc>
+  <rcc rId="978" sId="2">
+    <oc r="B40" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B40"/>
+  </rcc>
+  <rcc rId="979" sId="2">
+    <oc r="B41" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B41"/>
+  </rcc>
+  <rcc rId="980" sId="2">
+    <oc r="B42" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B42"/>
+  </rcc>
+  <rcc rId="981" sId="2">
+    <oc r="B43" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B43"/>
+  </rcc>
+  <rcc rId="982" sId="2">
+    <oc r="B44" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B44"/>
+  </rcc>
+  <rcc rId="983" sId="2">
+    <oc r="B45" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B45"/>
+  </rcc>
+  <rcc rId="984" sId="2">
+    <oc r="B46" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B46"/>
+  </rcc>
+  <rcc rId="985" sId="2">
+    <oc r="B47" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B47"/>
+  </rcc>
+  <rcc rId="986" sId="2">
+    <oc r="B48" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B48"/>
+  </rcc>
+  <rcc rId="987" sId="2">
+    <oc r="B49" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B49"/>
+  </rcc>
+  <rcc rId="988" sId="2">
+    <oc r="B50" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B50"/>
+  </rcc>
+  <rcc rId="989" sId="2">
+    <oc r="B51" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B51"/>
+  </rcc>
+  <rcc rId="990" sId="2">
+    <oc r="B52" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B52"/>
+  </rcc>
+  <rcc rId="991" sId="2">
+    <oc r="B53" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B53"/>
+  </rcc>
+  <rcc rId="992" sId="2">
+    <oc r="B54" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B54"/>
+  </rcc>
+  <rcc rId="993" sId="2">
+    <oc r="B55" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B55"/>
+  </rcc>
+  <rcc rId="994" sId="2">
+    <oc r="B56" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B56"/>
+  </rcc>
+  <rcc rId="995" sId="2">
+    <oc r="B57" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B57"/>
+  </rcc>
+  <rcc rId="996" sId="2">
+    <oc r="B58" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B58"/>
+  </rcc>
+  <rcc rId="997" sId="2">
+    <oc r="B59" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B59"/>
+  </rcc>
+  <rcc rId="998" sId="2">
+    <oc r="B60" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B60"/>
+  </rcc>
+  <rcc rId="999" sId="2">
+    <oc r="B61" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B61"/>
+  </rcc>
+  <rcc rId="1000" sId="2">
+    <oc r="B62" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B62"/>
+  </rcc>
+  <rcc rId="1001" sId="2">
+    <oc r="B63" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B63"/>
+  </rcc>
+  <rcc rId="1002" sId="2">
+    <oc r="B64" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B64"/>
+  </rcc>
+  <rcc rId="1003" sId="2">
+    <oc r="B65" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B65"/>
+  </rcc>
+  <rcc rId="1004" sId="2">
+    <oc r="B66" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B66"/>
+  </rcc>
+  <rcc rId="1005" sId="2">
+    <oc r="B67" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B67"/>
+  </rcc>
+  <rcc rId="1006" sId="2">
+    <oc r="B68" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B68"/>
+  </rcc>
+  <rcc rId="1007" sId="2">
+    <oc r="B69" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B69"/>
+  </rcc>
+  <rcc rId="1008" sId="2">
+    <oc r="B70" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B70"/>
+  </rcc>
+  <rcc rId="1009" sId="2">
+    <oc r="B71" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B71"/>
+  </rcc>
+  <rcc rId="1010" sId="2">
+    <oc r="B72" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B72"/>
+  </rcc>
+  <rcc rId="1011" sId="2">
+    <oc r="B73" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B73"/>
+  </rcc>
+  <rcc rId="1012" sId="2">
+    <oc r="B74" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B74"/>
+  </rcc>
+  <rcc rId="1013" sId="2">
+    <oc r="B75" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B75"/>
+  </rcc>
+  <rcc rId="1014" sId="2">
+    <oc r="B76" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B76"/>
+  </rcc>
+  <rcc rId="1015" sId="2">
+    <oc r="B77" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B77"/>
+  </rcc>
+  <rcc rId="1016" sId="2">
+    <oc r="B78" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B78"/>
+  </rcc>
+  <rcc rId="1017" sId="2">
+    <oc r="B79" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B79"/>
+  </rcc>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="delete"/>
+  <rdn rId="0" localSheetId="2" customView="1" name="Z_E811CF45_D5B3_4449_84AE_1514F9E9258F_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>case!$A$2:$AD$2</formula>
+    <oldFormula>case!$A$2:$AD$2</oldFormula>
+  </rdn>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="add"/>
+</revisions>
 </file>
 
 <file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11715,7 +12963,39 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/revisionLog9.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="857" sId="2">
+    <nc r="A82" t="inlineStr">
+      <is>
+        <t>80</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="858" sId="2">
+    <nc r="D82" t="inlineStr">
+      <is>
+        <t>Jedi</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="859" sId="2">
+    <nc r="E82" t="inlineStr">
+      <is>
+        <t>HDL_syntax/02_Jedi/security_flow/12_security</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="delete"/>
+  <rdn rId="0" localSheetId="2" customView="1" name="Z_E811CF45_D5B3_4449_84AE_1514F9E9258F_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>case!$A$2:$AD$2</formula>
+    <oldFormula>case!$A$2:$AD$2</oldFormula>
+  </rdn>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
 <users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
 </file>
 
@@ -12038,7 +13318,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -12072,7 +13352,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>270</v>
+        <v>433</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -12093,8 +13373,8 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="BrxOpSv5Qn+u2wRjM+utC6UYLrvUI+Gay+w6zPQp8zz+/5I1udizjqbZ6brqgp9h1Ud3zJVEOn/q/bgrm9i81A==" saltValue="wt9VphKaQ5GnARCLMZGRjA==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <customSheetViews>
-    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
-      <selection activeCell="B35" sqref="B35"/>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+      <selection activeCell="B12" sqref="B12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -12103,8 +13383,8 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
-      <selection activeCell="B12" sqref="B12"/>
+    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
+      <selection activeCell="B35" sqref="B35"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
@@ -12117,10 +13397,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD81"/>
+  <dimension ref="A1:AD82"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="A2" sqref="A2"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -12286,138 +13566,138 @@
     </row>
     <row r="3" spans="1:30" ht="15.75" thickTop="1">
       <c r="A3" s="18" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F3" s="18">
         <v>2</v>
       </c>
       <c r="S3" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="4" spans="1:30">
       <c r="A4" s="18" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="F4" s="18">
         <v>2</v>
       </c>
       <c r="S4" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="5" spans="1:30">
       <c r="A5" s="18" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="F5" s="18">
         <v>2</v>
       </c>
       <c r="S5" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="6" spans="1:30">
       <c r="A6" s="18" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F6" s="18">
         <v>2</v>
       </c>
       <c r="S6" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="7" spans="1:30">
       <c r="A7" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="F7" s="18">
         <v>2</v>
       </c>
       <c r="S7" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="8" spans="1:30">
       <c r="A8" s="18" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F8" s="18">
         <v>2</v>
       </c>
       <c r="S8" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="9" spans="1:30">
       <c r="A9" s="18" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="F9" s="18">
         <v>2</v>
       </c>
       <c r="S9" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="10" spans="1:30">
       <c r="A10" s="18" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="F10" s="18">
         <v>2</v>
       </c>
       <c r="S10" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="11" spans="1:30">
@@ -12425,1218 +13705,1235 @@
         <v>266</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F11" s="18">
         <v>2</v>
       </c>
       <c r="S11" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="12" spans="1:30">
       <c r="A12" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="F12" s="18">
         <v>2</v>
       </c>
       <c r="S12" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="13" spans="1:30">
       <c r="A13" s="18" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="F13" s="18">
         <v>2</v>
       </c>
       <c r="S13" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="14" spans="1:30">
       <c r="A14" s="18" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F14" s="18">
         <v>2</v>
       </c>
       <c r="S14" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="15" spans="1:30">
       <c r="A15" s="18" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F15" s="18">
         <v>2</v>
       </c>
       <c r="S15" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="16" spans="1:30">
       <c r="A16" s="18" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F16" s="18">
         <v>2</v>
       </c>
       <c r="S16" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="17" spans="1:19">
       <c r="A17" s="18" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F17" s="18">
         <v>2</v>
       </c>
       <c r="S17" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="18" spans="1:19">
       <c r="A18" s="18" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F18" s="18">
         <v>2</v>
       </c>
       <c r="S18" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="19" spans="1:19">
       <c r="A19" s="18" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F19" s="18">
         <v>2</v>
       </c>
       <c r="S19" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="20" spans="1:19">
       <c r="A20" s="18" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="F20" s="18">
         <v>2</v>
       </c>
       <c r="S20" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="21" spans="1:19">
       <c r="A21" s="18" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="F21" s="18">
         <v>2</v>
       </c>
       <c r="S21" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="22" spans="1:19">
       <c r="A22" s="18" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E22" s="18" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="F22" s="18">
         <v>2</v>
       </c>
       <c r="S22" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="23" spans="1:19">
       <c r="A23" s="18" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F23" s="18">
         <v>2</v>
       </c>
       <c r="S23" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="24" spans="1:19">
       <c r="A24" s="18" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D24" s="18" t="s">
+        <v>348</v>
+      </c>
+      <c r="E24" s="18" t="s">
         <v>349</v>
-      </c>
-      <c r="E24" s="18" t="s">
-        <v>350</v>
       </c>
       <c r="F24" s="18">
         <v>2</v>
       </c>
       <c r="S24" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="25" spans="1:19">
       <c r="A25" s="18" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F25" s="18">
         <v>2</v>
       </c>
       <c r="S25" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="26" spans="1:19">
       <c r="A26" s="18" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E26" s="18" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F26" s="18">
         <v>2</v>
       </c>
       <c r="S26" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="27" spans="1:19">
       <c r="A27" s="18" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F27" s="18">
         <v>2</v>
       </c>
       <c r="S27" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="28" spans="1:19">
       <c r="A28" s="18" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D28" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="F28" s="18">
         <v>2</v>
       </c>
       <c r="S28" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="29" spans="1:19">
       <c r="A29" s="18" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E29" s="18" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F29" s="18">
         <v>2</v>
       </c>
       <c r="S29" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="30" spans="1:19">
       <c r="A30" s="18" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D30" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F30" s="18">
         <v>2</v>
       </c>
       <c r="S30" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="31" spans="1:19">
       <c r="A31" s="18" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E31" s="18" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F31" s="18">
         <v>2</v>
       </c>
       <c r="S31" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="32" spans="1:19">
       <c r="A32" s="18" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E32" s="18" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F32" s="18">
         <v>2</v>
       </c>
       <c r="S32" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="33" spans="1:19">
       <c r="A33" s="18" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E33" s="18" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F33" s="18">
         <v>2</v>
       </c>
       <c r="S33" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="34" spans="1:19">
       <c r="A34" s="18" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D34" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E34" s="18" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="F34" s="18">
         <v>2</v>
       </c>
       <c r="S34" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="35" spans="1:19">
       <c r="A35" s="18" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D35" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E35" s="18" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F35" s="18">
         <v>2</v>
       </c>
       <c r="S35" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="36" spans="1:19">
       <c r="A36" s="18" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D36" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E36" s="18" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F36" s="18">
         <v>2</v>
       </c>
       <c r="S36" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="37" spans="1:19">
       <c r="A37" s="18" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E37" s="18" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F37" s="18">
         <v>2</v>
       </c>
       <c r="S37" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="38" spans="1:19">
       <c r="A38" s="18" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E38" s="18" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F38" s="18">
         <v>2</v>
       </c>
       <c r="S38" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="39" spans="1:19">
       <c r="A39" s="18" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E39" s="18" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F39" s="18">
         <v>2</v>
       </c>
       <c r="S39" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="40" spans="1:19">
       <c r="A40" s="18" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D40" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E40" s="18" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F40" s="18">
         <v>2</v>
       </c>
       <c r="S40" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="41" spans="1:19">
       <c r="A41" s="18" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D41" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E41" s="18" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F41" s="18">
         <v>2</v>
       </c>
       <c r="S41" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="42" spans="1:19">
       <c r="A42" s="18" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D42" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E42" s="18" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F42" s="18">
         <v>2</v>
       </c>
       <c r="S42" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="43" spans="1:19">
       <c r="A43" s="18" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D43" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E43" s="18" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F43" s="18">
         <v>2</v>
       </c>
       <c r="S43" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="44" spans="1:19">
       <c r="A44" s="18" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D44" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E44" s="18" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F44" s="18">
         <v>2</v>
       </c>
       <c r="S44" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="45" spans="1:19">
       <c r="A45" s="18" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D45" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E45" s="18" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F45" s="18">
         <v>2</v>
       </c>
       <c r="S45" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="46" spans="1:19">
       <c r="A46" s="18" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D46" s="18" t="s">
+        <v>371</v>
+      </c>
+      <c r="E46" s="18" t="s">
         <v>372</v>
-      </c>
-      <c r="E46" s="18" t="s">
-        <v>373</v>
       </c>
       <c r="F46" s="18">
         <v>2</v>
       </c>
       <c r="S46" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="47" spans="1:19">
       <c r="A47" s="18" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D47" s="18" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E47" s="18" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F47" s="18">
         <v>2</v>
       </c>
       <c r="S47" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="48" spans="1:19">
       <c r="A48" s="18" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D48" s="18" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E48" s="18" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F48" s="18">
         <v>2</v>
       </c>
       <c r="S48" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="49" spans="1:19">
       <c r="A49" s="18" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D49" s="18" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E49" s="18" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F49" s="18">
         <v>2</v>
       </c>
       <c r="S49" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="50" spans="1:19">
       <c r="A50" s="18" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D50" s="18" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E50" s="18" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F50" s="18">
         <v>2</v>
       </c>
       <c r="S50" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="51" spans="1:19">
       <c r="A51" s="18" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D51" s="18" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E51" s="18" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F51" s="18">
         <v>2</v>
       </c>
       <c r="S51" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="52" spans="1:19">
       <c r="A52" s="18" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D52" s="18" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E52" s="18" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F52" s="18">
         <v>2</v>
       </c>
       <c r="S52" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="53" spans="1:19">
       <c r="A53" s="18" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D53" s="18" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E53" s="18" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="F53" s="18">
         <v>2</v>
       </c>
       <c r="S53" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="54" spans="1:19">
       <c r="A54" s="18" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D54" s="18" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E54" s="18" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F54" s="18">
         <v>2</v>
       </c>
       <c r="S54" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="55" spans="1:19">
       <c r="A55" s="18" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D55" s="18" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E55" s="18" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F55" s="18">
         <v>2</v>
       </c>
       <c r="S55" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="56" spans="1:19">
       <c r="A56" s="18" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D56" s="18" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E56" s="18" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="F56" s="18">
         <v>2</v>
       </c>
       <c r="S56" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="57" spans="1:19">
       <c r="A57" s="18" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D57" s="18" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E57" s="18" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F57" s="18">
         <v>2</v>
       </c>
       <c r="S57" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="58" spans="1:19">
       <c r="A58" s="18" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D58" s="18" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E58" s="18" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F58" s="18">
         <v>2</v>
       </c>
       <c r="S58" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="59" spans="1:19">
       <c r="A59" s="18" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D59" s="18" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E59" s="18" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F59" s="18">
         <v>2</v>
       </c>
       <c r="S59" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="60" spans="1:19">
       <c r="A60" s="18" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D60" s="18" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E60" s="18" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="F60" s="18">
         <v>2</v>
       </c>
       <c r="S60" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="61" spans="1:19">
       <c r="A61" s="18" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D61" s="18" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E61" s="18" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F61" s="18">
         <v>2</v>
       </c>
       <c r="S61" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="62" spans="1:19">
       <c r="A62" s="18" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D62" s="18" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E62" s="18" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F62" s="18">
         <v>2</v>
       </c>
       <c r="S62" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="63" spans="1:19">
       <c r="A63" s="18" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D63" s="18" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E63" s="18" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="F63" s="18">
         <v>2</v>
       </c>
       <c r="S63" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="64" spans="1:19">
       <c r="A64" s="18" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D64" s="18" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E64" s="18" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F64" s="18">
         <v>2</v>
       </c>
       <c r="S64" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="65" spans="1:19">
       <c r="A65" s="18" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D65" s="18" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E65" s="18" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F65" s="18">
         <v>2</v>
       </c>
       <c r="S65" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="66" spans="1:19">
       <c r="A66" s="18" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D66" s="18" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E66" s="18" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F66" s="18">
         <v>2</v>
       </c>
       <c r="S66" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="67" spans="1:19">
       <c r="A67" s="18" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D67" s="18" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E67" s="18" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F67" s="18">
         <v>2</v>
       </c>
       <c r="S67" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="68" spans="1:19">
       <c r="A68" s="18" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D68" s="18" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E68" s="18" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F68" s="18">
         <v>2</v>
       </c>
       <c r="S68" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="69" spans="1:19">
       <c r="A69" s="18" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D69" s="18" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E69" s="18" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F69" s="18">
         <v>2</v>
       </c>
       <c r="S69" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="70" spans="1:19">
       <c r="A70" s="18" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D70" s="18" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E70" s="18" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F70" s="18">
         <v>2</v>
       </c>
       <c r="S70" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="71" spans="1:19">
       <c r="A71" s="18" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D71" s="18" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E71" s="18" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="F71" s="18">
         <v>2</v>
       </c>
       <c r="S71" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="72" spans="1:19">
       <c r="A72" s="18" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D72" s="18" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E72" s="18" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F72" s="18">
         <v>2</v>
       </c>
       <c r="S72" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="73" spans="1:19">
       <c r="A73" s="18" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D73" s="18" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E73" s="18" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F73" s="18">
         <v>2</v>
       </c>
       <c r="S73" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="74" spans="1:19">
       <c r="A74" s="18" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D74" s="18" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E74" s="18" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F74" s="18">
         <v>2</v>
       </c>
       <c r="S74" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="75" spans="1:19">
       <c r="A75" s="18" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D75" s="18" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E75" s="18" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="F75" s="18">
         <v>2</v>
       </c>
       <c r="S75" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="76" spans="1:19">
       <c r="A76" s="18" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D76" s="18" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E76" s="18" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F76" s="18">
         <v>2</v>
       </c>
       <c r="S76" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="77" spans="1:19">
       <c r="A77" s="18" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D77" s="18" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E77" s="18" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="F77" s="18">
         <v>2</v>
       </c>
       <c r="S77" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="78" spans="1:19">
       <c r="A78" s="18" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D78" s="18" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E78" s="18" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F78" s="18">
         <v>2</v>
       </c>
       <c r="S78" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="79" spans="1:19">
       <c r="A79" s="18" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D79" s="18" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E79" s="18" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F79" s="18">
         <v>2</v>
       </c>
       <c r="S79" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="80" spans="1:19">
       <c r="A80" s="18" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D80" s="18" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E80" s="18" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="F80" s="18">
         <v>2</v>
       </c>
       <c r="S80" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="81" spans="1:19">
       <c r="A81" s="18" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D81" s="18" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E81" s="18" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="F81" s="18">
         <v>2</v>
       </c>
       <c r="S81" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
+      </c>
+    </row>
+    <row r="82" spans="1:19">
+      <c r="A82" s="18" t="s">
+        <v>431</v>
+      </c>
+      <c r="D82" s="18" t="s">
+        <v>371</v>
+      </c>
+      <c r="E82" s="18" t="s">
+        <v>432</v>
+      </c>
+      <c r="F82" s="18">
+        <v>2</v>
+      </c>
+      <c r="S82" s="18" t="s">
+        <v>429</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="4C55417S7/WEfM6p9p+2qxLa3pFuuwTQvkVS+xLflxPJ6JUMhmXb8UBi2EhWPKsWHpV7wPPZoM4Ci73L5pzjfA==" saltValue="OVPlytvnGy6tQU/SUgOtyg==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <autoFilter ref="A2:AD2"/>
   <customSheetViews>
-    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" scale="85" showAutoFilter="1">
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" showAutoFilter="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-      <autoFilter ref="A2:Y2"/>
+      <autoFilter ref="A2:AD2"/>
     </customSheetView>
     <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" scale="85" showAutoFilter="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
@@ -13645,12 +14942,12 @@
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
       <autoFilter ref="A2:Y2"/>
     </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="55" showAutoFilter="1">
-      <pane xSplit="1" ySplit="2" topLeftCell="D15" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="M21" sqref="M21"/>
+    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" scale="85" showAutoFilter="1">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
-      <autoFilter ref="A2:AD2"/>
+      <autoFilter ref="A2:Y2"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="2">
@@ -13791,17 +15088,17 @@
       <c r="E109" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="F109" s="73" t="s">
+      <c r="F109" s="93" t="s">
         <v>64</v>
       </c>
-      <c r="G109" s="74"/>
-      <c r="H109" s="74"/>
-      <c r="I109" s="74"/>
-      <c r="J109" s="74"/>
-      <c r="K109" s="74"/>
-      <c r="L109" s="74"/>
-      <c r="M109" s="74"/>
-      <c r="N109" s="75"/>
+      <c r="G109" s="94"/>
+      <c r="H109" s="94"/>
+      <c r="I109" s="94"/>
+      <c r="J109" s="94"/>
+      <c r="K109" s="94"/>
+      <c r="L109" s="94"/>
+      <c r="M109" s="94"/>
+      <c r="N109" s="95"/>
     </row>
     <row r="110" spans="1:14">
       <c r="A110" s="6" t="s">
@@ -14639,7 +15936,7 @@
       <c r="A144" s="41">
         <v>1</v>
       </c>
-      <c r="B144" s="76" t="s">
+      <c r="B144" s="96" t="s">
         <v>122</v>
       </c>
       <c r="C144" s="39" t="s">
@@ -14665,7 +15962,7 @@
       <c r="A145" s="41">
         <v>2</v>
       </c>
-      <c r="B145" s="77"/>
+      <c r="B145" s="97"/>
       <c r="C145" s="39" t="s">
         <v>128</v>
       </c>
@@ -14687,7 +15984,7 @@
       <c r="A146" s="59">
         <v>3</v>
       </c>
-      <c r="B146" s="77"/>
+      <c r="B146" s="97"/>
       <c r="C146" s="39" t="s">
         <v>9</v>
       </c>
@@ -14705,7 +16002,7 @@
       <c r="A147" s="59">
         <v>4</v>
       </c>
-      <c r="B147" s="77"/>
+      <c r="B147" s="97"/>
       <c r="C147" s="60" t="s">
         <v>256</v>
       </c>
@@ -14727,7 +16024,7 @@
       <c r="A148" s="59">
         <v>5</v>
       </c>
-      <c r="B148" s="77"/>
+      <c r="B148" s="97"/>
       <c r="C148" s="39" t="s">
         <v>253</v>
       </c>
@@ -14747,7 +16044,7 @@
       <c r="A149" s="59">
         <v>6</v>
       </c>
-      <c r="B149" s="77"/>
+      <c r="B149" s="97"/>
       <c r="C149" s="60" t="s">
         <v>254</v>
       </c>
@@ -14769,7 +16066,7 @@
       <c r="A150" s="59">
         <v>7</v>
       </c>
-      <c r="B150" s="77"/>
+      <c r="B150" s="97"/>
       <c r="C150" s="39" t="s">
         <v>130</v>
       </c>
@@ -14791,7 +16088,7 @@
       <c r="A151" s="59">
         <v>8</v>
       </c>
-      <c r="B151" s="77"/>
+      <c r="B151" s="97"/>
       <c r="C151" s="39" t="s">
         <v>246</v>
       </c>
@@ -14813,7 +16110,7 @@
       <c r="A152" s="59">
         <v>9</v>
       </c>
-      <c r="B152" s="77"/>
+      <c r="B152" s="97"/>
       <c r="C152" s="39" t="s">
         <v>55</v>
       </c>
@@ -14837,7 +16134,7 @@
       <c r="A153" s="59">
         <v>10</v>
       </c>
-      <c r="B153" s="78"/>
+      <c r="B153" s="83"/>
       <c r="C153" s="39" t="s">
         <v>136</v>
       </c>
@@ -14859,7 +16156,7 @@
       <c r="A154" s="59">
         <v>11</v>
       </c>
-      <c r="B154" s="72" t="s">
+      <c r="B154" s="79" t="s">
         <v>139</v>
       </c>
       <c r="C154" s="39" t="s">
@@ -14885,7 +16182,7 @@
       <c r="A155" s="59">
         <v>12</v>
       </c>
-      <c r="B155" s="72"/>
+      <c r="B155" s="79"/>
       <c r="C155" s="39" t="s">
         <v>247</v>
       </c>
@@ -14909,7 +16206,7 @@
       <c r="A156" s="59">
         <v>13</v>
       </c>
-      <c r="B156" s="76" t="s">
+      <c r="B156" s="96" t="s">
         <v>143</v>
       </c>
       <c r="C156" s="39" t="s">
@@ -14933,7 +16230,7 @@
       <c r="A157" s="59">
         <v>14</v>
       </c>
-      <c r="B157" s="78"/>
+      <c r="B157" s="83"/>
       <c r="C157" s="39" t="s">
         <v>146</v>
       </c>
@@ -14953,7 +16250,7 @@
       <c r="A158" s="59">
         <v>15</v>
       </c>
-      <c r="B158" s="72" t="s">
+      <c r="B158" s="79" t="s">
         <v>148</v>
       </c>
       <c r="C158" s="39" t="s">
@@ -14977,7 +16274,7 @@
       <c r="A159" s="59">
         <v>16</v>
       </c>
-      <c r="B159" s="72"/>
+      <c r="B159" s="79"/>
       <c r="C159" s="39" t="s">
         <v>152</v>
       </c>
@@ -14997,7 +16294,7 @@
       <c r="A160" s="59">
         <v>17</v>
       </c>
-      <c r="B160" s="72"/>
+      <c r="B160" s="79"/>
       <c r="C160" s="39" t="s">
         <v>153</v>
       </c>
@@ -15017,7 +16314,7 @@
       <c r="A161" s="59">
         <v>18</v>
       </c>
-      <c r="B161" s="72"/>
+      <c r="B161" s="79"/>
       <c r="C161" s="39" t="s">
         <v>154</v>
       </c>
@@ -15037,7 +16334,7 @@
       <c r="A162" s="59">
         <v>19</v>
       </c>
-      <c r="B162" s="72"/>
+      <c r="B162" s="79"/>
       <c r="C162" s="39" t="s">
         <v>155</v>
       </c>
@@ -15057,7 +16354,7 @@
       <c r="A163" s="59">
         <v>20</v>
       </c>
-      <c r="B163" s="72"/>
+      <c r="B163" s="79"/>
       <c r="C163" s="39" t="s">
         <v>156</v>
       </c>
@@ -15077,7 +16374,7 @@
       <c r="A164" s="59">
         <v>21</v>
       </c>
-      <c r="B164" s="72"/>
+      <c r="B164" s="79"/>
       <c r="C164" s="39" t="s">
         <v>157</v>
       </c>
@@ -15097,7 +16394,7 @@
       <c r="A165" s="59">
         <v>22</v>
       </c>
-      <c r="B165" s="72"/>
+      <c r="B165" s="79"/>
       <c r="C165" s="39" t="s">
         <v>158</v>
       </c>
@@ -15117,7 +16414,7 @@
       <c r="A166" s="59">
         <v>23</v>
       </c>
-      <c r="B166" s="72" t="s">
+      <c r="B166" s="79" t="s">
         <v>159</v>
       </c>
       <c r="C166" s="39" t="s">
@@ -15141,7 +16438,7 @@
       <c r="A167" s="59">
         <v>24</v>
       </c>
-      <c r="B167" s="72"/>
+      <c r="B167" s="79"/>
       <c r="C167" s="39" t="s">
         <v>163</v>
       </c>
@@ -15163,7 +16460,7 @@
       <c r="A168" s="59">
         <v>25</v>
       </c>
-      <c r="B168" s="72"/>
+      <c r="B168" s="79"/>
       <c r="C168" s="39" t="s">
         <v>166</v>
       </c>
@@ -15185,7 +16482,7 @@
       <c r="A169" s="59">
         <v>26</v>
       </c>
-      <c r="B169" s="72" t="s">
+      <c r="B169" s="79" t="s">
         <v>169</v>
       </c>
       <c r="C169" s="39" t="s">
@@ -15209,7 +16506,7 @@
       <c r="A170" s="59">
         <v>27</v>
       </c>
-      <c r="B170" s="72"/>
+      <c r="B170" s="79"/>
       <c r="C170" s="39" t="s">
         <v>172</v>
       </c>
@@ -15231,7 +16528,7 @@
       <c r="A171" s="42">
         <v>28</v>
       </c>
-      <c r="B171" s="79"/>
+      <c r="B171" s="80"/>
       <c r="C171" s="40"/>
       <c r="D171" s="40"/>
       <c r="E171" s="40"/>
@@ -15267,11 +16564,11 @@
       <c r="B185" s="26" t="s">
         <v>178</v>
       </c>
-      <c r="C185" s="80" t="s">
+      <c r="C185" s="89" t="s">
         <v>43</v>
       </c>
-      <c r="D185" s="80"/>
-      <c r="E185" s="80"/>
+      <c r="D185" s="89"/>
+      <c r="E185" s="89"/>
       <c r="F185" s="34" t="s">
         <v>42</v>
       </c>
@@ -15280,17 +16577,17 @@
       </c>
     </row>
     <row r="186" spans="1:7">
-      <c r="A186" s="72" t="s">
+      <c r="A186" s="79" t="s">
         <v>180</v>
       </c>
-      <c r="B186" s="72" t="s">
+      <c r="B186" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="C186" s="81" t="s">
+      <c r="C186" s="90" t="s">
         <v>182</v>
       </c>
-      <c r="D186" s="81"/>
-      <c r="E186" s="81"/>
+      <c r="D186" s="90"/>
+      <c r="E186" s="90"/>
       <c r="F186" s="39" t="s">
         <v>183</v>
       </c>
@@ -15299,13 +16596,13 @@
       </c>
     </row>
     <row r="187" spans="1:7">
-      <c r="A187" s="72"/>
-      <c r="B187" s="72"/>
-      <c r="C187" s="82" t="s">
+      <c r="A187" s="79"/>
+      <c r="B187" s="79"/>
+      <c r="C187" s="91" t="s">
         <v>56</v>
       </c>
-      <c r="D187" s="82"/>
-      <c r="E187" s="82"/>
+      <c r="D187" s="91"/>
+      <c r="E187" s="91"/>
       <c r="F187" s="39" t="s">
         <v>185</v>
       </c>
@@ -15314,15 +16611,15 @@
       </c>
     </row>
     <row r="188" spans="1:7">
-      <c r="A188" s="72"/>
-      <c r="B188" s="72" t="s">
+      <c r="A188" s="79"/>
+      <c r="B188" s="79" t="s">
         <v>186</v>
       </c>
-      <c r="C188" s="83" t="s">
+      <c r="C188" s="92" t="s">
         <v>187</v>
       </c>
-      <c r="D188" s="83"/>
-      <c r="E188" s="83"/>
+      <c r="D188" s="92"/>
+      <c r="E188" s="92"/>
       <c r="F188" s="39" t="s">
         <v>183</v>
       </c>
@@ -15331,13 +16628,13 @@
       </c>
     </row>
     <row r="189" spans="1:7">
-      <c r="A189" s="72"/>
-      <c r="B189" s="72"/>
-      <c r="C189" s="83" t="s">
+      <c r="A189" s="79"/>
+      <c r="B189" s="79"/>
+      <c r="C189" s="92" t="s">
         <v>187</v>
       </c>
-      <c r="D189" s="83"/>
-      <c r="E189" s="83"/>
+      <c r="D189" s="92"/>
+      <c r="E189" s="92"/>
       <c r="F189" s="39" t="s">
         <v>185</v>
       </c>
@@ -15346,17 +16643,17 @@
       </c>
     </row>
     <row r="190" spans="1:7">
-      <c r="A190" s="84" t="s">
+      <c r="A190" s="77" t="s">
         <v>188</v>
       </c>
-      <c r="B190" s="72" t="s">
+      <c r="B190" s="79" t="s">
         <v>189</v>
       </c>
-      <c r="C190" s="72" t="s">
+      <c r="C190" s="79" t="s">
         <v>44</v>
       </c>
-      <c r="D190" s="72"/>
-      <c r="E190" s="72"/>
+      <c r="D190" s="79"/>
+      <c r="E190" s="79"/>
       <c r="F190" s="39" t="s">
         <v>183</v>
       </c>
@@ -15365,13 +16662,13 @@
       </c>
     </row>
     <row r="191" spans="1:7">
-      <c r="A191" s="84"/>
-      <c r="B191" s="72"/>
-      <c r="C191" s="72" t="s">
+      <c r="A191" s="77"/>
+      <c r="B191" s="79"/>
+      <c r="C191" s="79" t="s">
         <v>45</v>
       </c>
-      <c r="D191" s="72"/>
-      <c r="E191" s="72"/>
+      <c r="D191" s="79"/>
+      <c r="E191" s="79"/>
       <c r="F191" s="39" t="s">
         <v>185</v>
       </c>
@@ -15380,15 +16677,15 @@
       </c>
     </row>
     <row r="192" spans="1:7">
-      <c r="A192" s="84"/>
-      <c r="B192" s="72" t="s">
+      <c r="A192" s="77"/>
+      <c r="B192" s="79" t="s">
         <v>190</v>
       </c>
-      <c r="C192" s="72" t="s">
+      <c r="C192" s="79" t="s">
         <v>46</v>
       </c>
-      <c r="D192" s="72"/>
-      <c r="E192" s="72"/>
+      <c r="D192" s="79"/>
+      <c r="E192" s="79"/>
       <c r="F192" s="39" t="s">
         <v>183</v>
       </c>
@@ -15397,13 +16694,13 @@
       </c>
     </row>
     <row r="193" spans="1:7">
-      <c r="A193" s="84"/>
-      <c r="B193" s="72"/>
-      <c r="C193" s="72" t="s">
+      <c r="A193" s="77"/>
+      <c r="B193" s="79"/>
+      <c r="C193" s="79" t="s">
         <v>47</v>
       </c>
-      <c r="D193" s="72"/>
-      <c r="E193" s="72"/>
+      <c r="D193" s="79"/>
+      <c r="E193" s="79"/>
       <c r="F193" s="39" t="s">
         <v>185</v>
       </c>
@@ -15412,17 +16709,17 @@
       </c>
     </row>
     <row r="194" spans="1:7">
-      <c r="A194" s="84" t="s">
+      <c r="A194" s="77" t="s">
         <v>191</v>
       </c>
-      <c r="B194" s="72" t="s">
+      <c r="B194" s="79" t="s">
         <v>192</v>
       </c>
-      <c r="C194" s="72" t="s">
+      <c r="C194" s="79" t="s">
         <v>48</v>
       </c>
-      <c r="D194" s="72"/>
-      <c r="E194" s="72"/>
+      <c r="D194" s="79"/>
+      <c r="E194" s="79"/>
       <c r="F194" s="39" t="s">
         <v>183</v>
       </c>
@@ -15431,13 +16728,13 @@
       </c>
     </row>
     <row r="195" spans="1:7">
-      <c r="A195" s="84"/>
-      <c r="B195" s="72"/>
-      <c r="C195" s="72" t="s">
+      <c r="A195" s="77"/>
+      <c r="B195" s="79"/>
+      <c r="C195" s="79" t="s">
         <v>49</v>
       </c>
-      <c r="D195" s="72"/>
-      <c r="E195" s="72"/>
+      <c r="D195" s="79"/>
+      <c r="E195" s="79"/>
       <c r="F195" s="39" t="s">
         <v>185</v>
       </c>
@@ -15446,15 +16743,15 @@
       </c>
     </row>
     <row r="196" spans="1:7">
-      <c r="A196" s="84"/>
-      <c r="B196" s="72" t="s">
+      <c r="A196" s="77"/>
+      <c r="B196" s="79" t="s">
         <v>193</v>
       </c>
-      <c r="C196" s="72" t="s">
+      <c r="C196" s="79" t="s">
         <v>194</v>
       </c>
-      <c r="D196" s="72"/>
-      <c r="E196" s="72"/>
+      <c r="D196" s="79"/>
+      <c r="E196" s="79"/>
       <c r="F196" s="39" t="s">
         <v>183</v>
       </c>
@@ -15463,13 +16760,13 @@
       </c>
     </row>
     <row r="197" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A197" s="86"/>
-      <c r="B197" s="79"/>
-      <c r="C197" s="79" t="s">
+      <c r="A197" s="78"/>
+      <c r="B197" s="80"/>
+      <c r="C197" s="80" t="s">
         <v>195</v>
       </c>
-      <c r="D197" s="79"/>
-      <c r="E197" s="79"/>
+      <c r="D197" s="80"/>
+      <c r="E197" s="80"/>
       <c r="F197" s="40" t="s">
         <v>185</v>
       </c>
@@ -15508,12 +16805,12 @@
       <c r="A202" s="21" t="s">
         <v>197</v>
       </c>
-      <c r="B202" s="87" t="s">
+      <c r="B202" s="81" t="s">
         <v>198</v>
       </c>
-      <c r="C202" s="87"/>
-      <c r="D202" s="87"/>
-      <c r="E202" s="87"/>
+      <c r="C202" s="81"/>
+      <c r="D202" s="81"/>
+      <c r="E202" s="81"/>
       <c r="F202" s="22" t="s">
         <v>199</v>
       </c>
@@ -15525,12 +16822,12 @@
       <c r="A203" s="35" t="s">
         <v>201</v>
       </c>
-      <c r="B203" s="88" t="s">
+      <c r="B203" s="82" t="s">
         <v>202</v>
       </c>
-      <c r="C203" s="78"/>
-      <c r="D203" s="78"/>
-      <c r="E203" s="78"/>
+      <c r="C203" s="83"/>
+      <c r="D203" s="83"/>
+      <c r="E203" s="83"/>
       <c r="F203" s="36" t="s">
         <v>203</v>
       </c>
@@ -15542,12 +16839,12 @@
       <c r="A204" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="B204" s="89" t="s">
+      <c r="B204" s="84" t="s">
         <v>205</v>
       </c>
-      <c r="C204" s="90"/>
-      <c r="D204" s="90"/>
-      <c r="E204" s="91"/>
+      <c r="C204" s="85"/>
+      <c r="D204" s="85"/>
+      <c r="E204" s="86"/>
       <c r="F204" s="10" t="s">
         <v>184</v>
       </c>
@@ -15559,12 +16856,12 @@
       <c r="A205" s="45" t="s">
         <v>230</v>
       </c>
-      <c r="B205" s="89" t="s">
+      <c r="B205" s="84" t="s">
         <v>233</v>
       </c>
-      <c r="C205" s="90"/>
-      <c r="D205" s="90"/>
-      <c r="E205" s="91"/>
+      <c r="C205" s="85"/>
+      <c r="D205" s="85"/>
+      <c r="E205" s="86"/>
       <c r="F205" s="46" t="s">
         <v>231</v>
       </c>
@@ -15576,12 +16873,12 @@
       <c r="A206" s="12" t="s">
         <v>232</v>
       </c>
-      <c r="B206" s="92" t="s">
+      <c r="B206" s="87" t="s">
         <v>234</v>
       </c>
-      <c r="C206" s="79"/>
-      <c r="D206" s="79"/>
-      <c r="E206" s="79"/>
+      <c r="C206" s="80"/>
+      <c r="D206" s="80"/>
+      <c r="E206" s="80"/>
       <c r="F206" s="13" t="s">
         <v>184</v>
       </c>
@@ -15626,11 +16923,11 @@
       <c r="C211" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="D211" s="93" t="s">
+      <c r="D211" s="88" t="s">
         <v>53</v>
       </c>
-      <c r="E211" s="93"/>
-      <c r="F211" s="93"/>
+      <c r="E211" s="88"/>
+      <c r="F211" s="88"/>
       <c r="G211" s="32"/>
     </row>
     <row r="212" spans="1:7">
@@ -15643,11 +16940,11 @@
       <c r="C212" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="D212" s="85" t="s">
+      <c r="D212" s="72" t="s">
         <v>54</v>
       </c>
-      <c r="E212" s="85"/>
-      <c r="F212" s="85"/>
+      <c r="E212" s="72"/>
+      <c r="F212" s="72"/>
       <c r="G212" s="24"/>
     </row>
     <row r="213" spans="1:7">
@@ -15660,11 +16957,11 @@
       <c r="C213" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="D213" s="85" t="s">
+      <c r="D213" s="72" t="s">
         <v>209</v>
       </c>
-      <c r="E213" s="85"/>
-      <c r="F213" s="85"/>
+      <c r="E213" s="72"/>
+      <c r="F213" s="72"/>
       <c r="G213" s="24"/>
     </row>
     <row r="214" spans="1:7">
@@ -15677,11 +16974,11 @@
       <c r="C214" s="39" t="s">
         <v>210</v>
       </c>
-      <c r="D214" s="85" t="s">
+      <c r="D214" s="72" t="s">
         <v>211</v>
       </c>
-      <c r="E214" s="85"/>
-      <c r="F214" s="85"/>
+      <c r="E214" s="72"/>
+      <c r="F214" s="72"/>
       <c r="G214" s="24"/>
     </row>
     <row r="215" spans="1:7">
@@ -15694,11 +16991,11 @@
       <c r="C215" s="44" t="s">
         <v>210</v>
       </c>
-      <c r="D215" s="85" t="s">
+      <c r="D215" s="72" t="s">
         <v>222</v>
       </c>
-      <c r="E215" s="85"/>
-      <c r="F215" s="85"/>
+      <c r="E215" s="72"/>
+      <c r="F215" s="72"/>
       <c r="G215" s="24"/>
     </row>
     <row r="216" spans="1:7">
@@ -15711,11 +17008,11 @@
       <c r="C216" s="39" t="s">
         <v>236</v>
       </c>
-      <c r="D216" s="85" t="s">
+      <c r="D216" s="72" t="s">
         <v>235</v>
       </c>
-      <c r="E216" s="85"/>
-      <c r="F216" s="85"/>
+      <c r="E216" s="72"/>
+      <c r="F216" s="72"/>
       <c r="G216" s="24"/>
     </row>
     <row r="217" spans="1:7">
@@ -15728,11 +17025,11 @@
       <c r="C217" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="D217" s="95" t="s">
+      <c r="D217" s="74" t="s">
         <v>237</v>
       </c>
-      <c r="E217" s="96"/>
-      <c r="F217" s="97"/>
+      <c r="E217" s="75"/>
+      <c r="F217" s="76"/>
       <c r="G217" s="53"/>
     </row>
     <row r="218" spans="1:7">
@@ -15745,11 +17042,11 @@
       <c r="C218" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="D218" s="95" t="s">
+      <c r="D218" s="74" t="s">
         <v>238</v>
       </c>
-      <c r="E218" s="96"/>
-      <c r="F218" s="97"/>
+      <c r="E218" s="75"/>
+      <c r="F218" s="76"/>
       <c r="G218" s="53"/>
     </row>
     <row r="219" spans="1:7">
@@ -15762,11 +17059,11 @@
       <c r="C219" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="D219" s="95" t="s">
+      <c r="D219" s="74" t="s">
         <v>251</v>
       </c>
-      <c r="E219" s="96"/>
-      <c r="F219" s="97"/>
+      <c r="E219" s="75"/>
+      <c r="F219" s="76"/>
       <c r="G219" s="53"/>
     </row>
     <row r="220" spans="1:7">
@@ -15813,11 +17110,11 @@
       <c r="C222" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="D222" s="94" t="s">
+      <c r="D222" s="73" t="s">
         <v>264</v>
       </c>
-      <c r="E222" s="94"/>
-      <c r="F222" s="94"/>
+      <c r="E222" s="73"/>
+      <c r="F222" s="73"/>
       <c r="G222" s="25"/>
     </row>
   </sheetData>
@@ -15830,14 +17127,28 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="44">
-    <mergeCell ref="D213:F213"/>
-    <mergeCell ref="D214:F214"/>
-    <mergeCell ref="D215:F215"/>
-    <mergeCell ref="D216:F216"/>
-    <mergeCell ref="D222:F222"/>
-    <mergeCell ref="D217:F217"/>
-    <mergeCell ref="D218:F218"/>
-    <mergeCell ref="D219:F219"/>
+    <mergeCell ref="B166:B168"/>
+    <mergeCell ref="F109:N109"/>
+    <mergeCell ref="B144:B153"/>
+    <mergeCell ref="B154:B155"/>
+    <mergeCell ref="B156:B157"/>
+    <mergeCell ref="B158:B165"/>
+    <mergeCell ref="B169:B171"/>
+    <mergeCell ref="C185:E185"/>
+    <mergeCell ref="A186:A189"/>
+    <mergeCell ref="B186:B187"/>
+    <mergeCell ref="C186:E186"/>
+    <mergeCell ref="C187:E187"/>
+    <mergeCell ref="B188:B189"/>
+    <mergeCell ref="C188:E188"/>
+    <mergeCell ref="C189:E189"/>
+    <mergeCell ref="A190:A193"/>
+    <mergeCell ref="B190:B191"/>
+    <mergeCell ref="C190:E190"/>
+    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="B192:B193"/>
+    <mergeCell ref="C192:E192"/>
+    <mergeCell ref="C193:E193"/>
     <mergeCell ref="D212:F212"/>
     <mergeCell ref="A194:A197"/>
     <mergeCell ref="B194:B195"/>
@@ -15852,28 +17163,14 @@
     <mergeCell ref="B206:E206"/>
     <mergeCell ref="D211:F211"/>
     <mergeCell ref="B205:E205"/>
-    <mergeCell ref="A190:A193"/>
-    <mergeCell ref="B190:B191"/>
-    <mergeCell ref="C190:E190"/>
-    <mergeCell ref="C191:E191"/>
-    <mergeCell ref="B192:B193"/>
-    <mergeCell ref="C192:E192"/>
-    <mergeCell ref="C193:E193"/>
-    <mergeCell ref="B169:B171"/>
-    <mergeCell ref="C185:E185"/>
-    <mergeCell ref="A186:A189"/>
-    <mergeCell ref="B186:B187"/>
-    <mergeCell ref="C186:E186"/>
-    <mergeCell ref="C187:E187"/>
-    <mergeCell ref="B188:B189"/>
-    <mergeCell ref="C188:E188"/>
-    <mergeCell ref="C189:E189"/>
-    <mergeCell ref="B166:B168"/>
-    <mergeCell ref="F109:N109"/>
-    <mergeCell ref="B144:B153"/>
-    <mergeCell ref="B154:B155"/>
-    <mergeCell ref="B156:B157"/>
-    <mergeCell ref="B158:B165"/>
+    <mergeCell ref="D213:F213"/>
+    <mergeCell ref="D214:F214"/>
+    <mergeCell ref="D215:F215"/>
+    <mergeCell ref="D216:F216"/>
+    <mergeCell ref="D222:F222"/>
+    <mergeCell ref="D217:F217"/>
+    <mergeCell ref="D218:F218"/>
+    <mergeCell ref="D219:F219"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15897,15 +17194,15 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
-      <selection activeCell="E26" sqref="E26"/>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
       <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
+      <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>

<commit_message>
i264--reveal suite file update
</commit_message>
<xml_diff>
--- a/tmp_client/doc/TMP_EIT_suites/debug_10_reveal_inserter_all.xlsx
+++ b/tmp_client/doc/TMP_EIT_suites/debug_10_reveal_inserter_all.xlsx
@@ -26,15 +26,15 @@
   </definedNames>
   <calcPr calcId="122211"/>
   <customWorkbookViews>
-    <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="2"/>
+    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
     <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" mergeInterval="0" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
-    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
+    <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="2"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="436">
   <si>
     <t>[suite_info]</t>
   </si>
@@ -1559,6 +1559,12 @@
   </si>
   <si>
     <t>radiant=ng2_1</t>
+  </si>
+  <si>
+    <t>81</t>
+  </si>
+  <si>
+    <t>HDL_syntax/02_Jedi/security_flow/tst_06_encrypt_sub_module_lse</t>
   </si>
 </sst>
 </file>
@@ -2854,30 +2860,46 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="24" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="25" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="26" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="22" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="37" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="35" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="38" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="44" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="39" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="44" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="44" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="41" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="21" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="22" xfId="41" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="33" xfId="41" applyBorder="1" applyAlignment="1">
@@ -2885,9 +2907,6 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="26" xfId="41" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="26" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="37" xfId="41" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2904,30 +2923,17 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="41" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="35" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="22" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="44" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="37" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="44" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="38" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="44" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="24" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="25" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="39" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="48">
@@ -5410,7 +5416,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{8E4B05B1-3E12-4F85-983B-CA42D07E19EC}" diskRevisions="1" revisionId="1018" version="13">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{AFF318DA-60AB-453A-B5B1-789997151B91}" diskRevisions="1" revisionId="1185" version="19">
   <header guid="{DB40D02A-1C38-451A-8E02-505A412F9BEE}" dateTime="2020-03-04T15:04:22" maxSheetId="5" userName="Jason Wang" r:id="rId1">
     <sheetIdMap count="4">
       <sheetId val="1"/>
@@ -5515,6 +5521,54 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
+  <header guid="{13988FB3-29F4-416F-A791-F3D0E836243F}" dateTime="2020-03-26T09:31:11" maxSheetId="5" userName="Jason Wang" r:id="rId14" minRId="1019" maxRId="1023">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{9A5AC6B4-C984-4CC5-AAC8-93D945B552FC}" dateTime="2020-03-26T09:31:55" maxSheetId="5" userName="Jason Wang" r:id="rId15" minRId="1025" maxRId="1102">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{CBB26E76-969F-4CBC-A7B7-64470846D666}" dateTime="2020-03-26T09:37:26" maxSheetId="5" userName="Jason Wang" r:id="rId16" minRId="1104" maxRId="1181">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{D7A16F27-9DCC-4662-8B37-377B3D5E452E}" dateTime="2020-03-26T09:37:29" maxSheetId="5" userName="Jason Wang" r:id="rId17">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{2AC07112-74DE-4AD0-9666-CD7A964E6CE2}" dateTime="2020-03-26T09:38:05" maxSheetId="5" userName="Jason Wang" r:id="rId18">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{AFF318DA-60AB-453A-B5B1-789997151B91}" dateTime="2020-03-26T09:38:12" maxSheetId="5" userName="Jason Wang" r:id="rId19">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -6715,6 +6769,1275 @@
     </oc>
     <nc r="B79"/>
   </rcc>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="delete"/>
+  <rdn rId="0" localSheetId="2" customView="1" name="Z_E811CF45_D5B3_4449_84AE_1514F9E9258F_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>case!$A$2:$AD$2</formula>
+    <oldFormula>case!$A$2:$AD$2</oldFormula>
+  </rdn>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog14.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1019" sId="2">
+    <nc r="A83" t="inlineStr">
+      <is>
+        <t>81</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1020" sId="2">
+    <nc r="D83" t="inlineStr">
+      <is>
+        <t>Jedi</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1021" sId="2">
+    <nc r="E83" t="inlineStr">
+      <is>
+        <t>HDL_syntax/02_Jedi/security_flow/tst_06_encrypt_sub_module_lse</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1022" sId="2" numFmtId="30">
+    <nc r="F83">
+      <v>2</v>
+    </nc>
+  </rcc>
+  <rcc rId="1023" sId="2">
+    <nc r="S83" t="inlineStr">
+      <is>
+        <t>reveal</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="delete"/>
+  <rdn rId="0" localSheetId="2" customView="1" name="Z_E811CF45_D5B3_4449_84AE_1514F9E9258F_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>case!$A$2:$AD$2</formula>
+    <oldFormula>case!$A$2:$AD$2</oldFormula>
+  </rdn>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog15.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1025" sId="2">
+    <nc r="B81" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1026" sId="2">
+    <nc r="B80" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1027" sId="2">
+    <nc r="B4" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1028" sId="2">
+    <nc r="B5" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1029" sId="2">
+    <nc r="B6" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1030" sId="2">
+    <nc r="B7" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1031" sId="2">
+    <nc r="B8" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1032" sId="2">
+    <nc r="B9" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1033" sId="2">
+    <nc r="B10" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1034" sId="2">
+    <nc r="B11" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1035" sId="2">
+    <nc r="B12" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1036" sId="2">
+    <nc r="B13" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1037" sId="2">
+    <nc r="B14" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1038" sId="2">
+    <nc r="B15" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1039" sId="2">
+    <nc r="B16" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1040" sId="2">
+    <nc r="B17" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1041" sId="2">
+    <nc r="B18" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1042" sId="2">
+    <nc r="B19" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1043" sId="2">
+    <nc r="B20" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1044" sId="2">
+    <nc r="B21" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1045" sId="2">
+    <nc r="B22" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1046" sId="2">
+    <nc r="B23" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1047" sId="2">
+    <nc r="B24" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1048" sId="2">
+    <nc r="B25" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1049" sId="2">
+    <nc r="B26" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1050" sId="2">
+    <nc r="B27" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1051" sId="2">
+    <nc r="B28" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1052" sId="2">
+    <nc r="B29" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1053" sId="2">
+    <nc r="B30" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1054" sId="2">
+    <nc r="B31" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1055" sId="2">
+    <nc r="B32" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1056" sId="2">
+    <nc r="B33" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1057" sId="2">
+    <nc r="B34" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1058" sId="2">
+    <nc r="B35" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1059" sId="2">
+    <nc r="B36" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1060" sId="2">
+    <nc r="B37" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1061" sId="2">
+    <nc r="B38" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1062" sId="2">
+    <nc r="B39" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1063" sId="2">
+    <nc r="B40" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1064" sId="2">
+    <nc r="B41" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1065" sId="2">
+    <nc r="B42" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1066" sId="2">
+    <nc r="B43" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1067" sId="2">
+    <nc r="B44" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1068" sId="2">
+    <nc r="B45" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1069" sId="2">
+    <nc r="B46" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1070" sId="2">
+    <nc r="B47" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1071" sId="2">
+    <nc r="B48" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1072" sId="2">
+    <nc r="B49" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1073" sId="2">
+    <nc r="B50" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1074" sId="2">
+    <nc r="B51" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1075" sId="2">
+    <nc r="B52" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1076" sId="2">
+    <nc r="B53" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1077" sId="2">
+    <nc r="B54" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1078" sId="2">
+    <nc r="B55" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1079" sId="2">
+    <nc r="B56" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1080" sId="2">
+    <nc r="B57" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1081" sId="2">
+    <nc r="B58" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1082" sId="2">
+    <nc r="B59" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1083" sId="2">
+    <nc r="B60" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1084" sId="2">
+    <nc r="B61" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1085" sId="2">
+    <nc r="B62" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1086" sId="2">
+    <nc r="B63" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1087" sId="2">
+    <nc r="B64" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1088" sId="2">
+    <nc r="B65" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1089" sId="2">
+    <nc r="B66" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1090" sId="2">
+    <nc r="B67" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1091" sId="2">
+    <nc r="B68" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1092" sId="2">
+    <nc r="B69" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1093" sId="2">
+    <nc r="B70" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1094" sId="2">
+    <nc r="B71" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1095" sId="2">
+    <nc r="B72" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1096" sId="2">
+    <nc r="B73" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1097" sId="2">
+    <nc r="B74" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1098" sId="2">
+    <nc r="B75" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1099" sId="2">
+    <nc r="B76" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1100" sId="2">
+    <nc r="B77" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1101" sId="2">
+    <nc r="B78" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1102" sId="2">
+    <nc r="B79" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="delete"/>
+  <rdn rId="0" localSheetId="2" customView="1" name="Z_E811CF45_D5B3_4449_84AE_1514F9E9258F_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>case!$A$2:$AD$2</formula>
+    <oldFormula>case!$A$2:$AD$2</oldFormula>
+  </rdn>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog16.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1104" sId="2">
+    <oc r="B4" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B4"/>
+  </rcc>
+  <rcc rId="1105" sId="2">
+    <oc r="B5" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B5"/>
+  </rcc>
+  <rcc rId="1106" sId="2">
+    <oc r="B6" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B6"/>
+  </rcc>
+  <rcc rId="1107" sId="2">
+    <oc r="B7" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B7"/>
+  </rcc>
+  <rcc rId="1108" sId="2">
+    <oc r="B8" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B8"/>
+  </rcc>
+  <rcc rId="1109" sId="2">
+    <oc r="B9" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B9"/>
+  </rcc>
+  <rcc rId="1110" sId="2">
+    <oc r="B10" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B10"/>
+  </rcc>
+  <rcc rId="1111" sId="2">
+    <oc r="B11" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B11"/>
+  </rcc>
+  <rcc rId="1112" sId="2">
+    <oc r="B12" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B12"/>
+  </rcc>
+  <rcc rId="1113" sId="2">
+    <oc r="B13" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B13"/>
+  </rcc>
+  <rcc rId="1114" sId="2">
+    <oc r="B14" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B14"/>
+  </rcc>
+  <rcc rId="1115" sId="2">
+    <oc r="B15" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B15"/>
+  </rcc>
+  <rcc rId="1116" sId="2">
+    <oc r="B16" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B16"/>
+  </rcc>
+  <rcc rId="1117" sId="2">
+    <oc r="B17" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B17"/>
+  </rcc>
+  <rcc rId="1118" sId="2">
+    <oc r="B18" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B18"/>
+  </rcc>
+  <rcc rId="1119" sId="2">
+    <oc r="B19" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B19"/>
+  </rcc>
+  <rcc rId="1120" sId="2">
+    <oc r="B20" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B20"/>
+  </rcc>
+  <rcc rId="1121" sId="2">
+    <oc r="B21" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B21"/>
+  </rcc>
+  <rcc rId="1122" sId="2">
+    <oc r="B22" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B22"/>
+  </rcc>
+  <rcc rId="1123" sId="2">
+    <oc r="B23" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B23"/>
+  </rcc>
+  <rcc rId="1124" sId="2">
+    <oc r="B24" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B24"/>
+  </rcc>
+  <rcc rId="1125" sId="2">
+    <oc r="B25" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B25"/>
+  </rcc>
+  <rcc rId="1126" sId="2">
+    <oc r="B26" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B26"/>
+  </rcc>
+  <rcc rId="1127" sId="2">
+    <oc r="B27" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B27"/>
+  </rcc>
+  <rcc rId="1128" sId="2">
+    <oc r="B28" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B28"/>
+  </rcc>
+  <rcc rId="1129" sId="2">
+    <oc r="B29" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B29"/>
+  </rcc>
+  <rcc rId="1130" sId="2">
+    <oc r="B30" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B30"/>
+  </rcc>
+  <rcc rId="1131" sId="2">
+    <oc r="B31" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B31"/>
+  </rcc>
+  <rcc rId="1132" sId="2">
+    <oc r="B32" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B32"/>
+  </rcc>
+  <rcc rId="1133" sId="2">
+    <oc r="B33" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B33"/>
+  </rcc>
+  <rcc rId="1134" sId="2">
+    <oc r="B34" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B34"/>
+  </rcc>
+  <rcc rId="1135" sId="2">
+    <oc r="B35" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B35"/>
+  </rcc>
+  <rcc rId="1136" sId="2">
+    <oc r="B36" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B36"/>
+  </rcc>
+  <rcc rId="1137" sId="2">
+    <oc r="B37" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B37"/>
+  </rcc>
+  <rcc rId="1138" sId="2">
+    <oc r="B38" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B38"/>
+  </rcc>
+  <rcc rId="1139" sId="2">
+    <oc r="B39" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B39"/>
+  </rcc>
+  <rcc rId="1140" sId="2">
+    <oc r="B40" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B40"/>
+  </rcc>
+  <rcc rId="1141" sId="2">
+    <oc r="B41" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B41"/>
+  </rcc>
+  <rcc rId="1142" sId="2">
+    <oc r="B42" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B42"/>
+  </rcc>
+  <rcc rId="1143" sId="2">
+    <oc r="B43" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B43"/>
+  </rcc>
+  <rcc rId="1144" sId="2">
+    <oc r="B44" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B44"/>
+  </rcc>
+  <rcc rId="1145" sId="2">
+    <oc r="B45" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B45"/>
+  </rcc>
+  <rcc rId="1146" sId="2">
+    <oc r="B46" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B46"/>
+  </rcc>
+  <rcc rId="1147" sId="2">
+    <oc r="B47" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B47"/>
+  </rcc>
+  <rcc rId="1148" sId="2">
+    <oc r="B48" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B48"/>
+  </rcc>
+  <rcc rId="1149" sId="2">
+    <oc r="B49" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B49"/>
+  </rcc>
+  <rcc rId="1150" sId="2">
+    <oc r="B50" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B50"/>
+  </rcc>
+  <rcc rId="1151" sId="2">
+    <oc r="B51" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B51"/>
+  </rcc>
+  <rcc rId="1152" sId="2">
+    <oc r="B52" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B52"/>
+  </rcc>
+  <rcc rId="1153" sId="2">
+    <oc r="B53" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B53"/>
+  </rcc>
+  <rcc rId="1154" sId="2">
+    <oc r="B54" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B54"/>
+  </rcc>
+  <rcc rId="1155" sId="2">
+    <oc r="B55" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B55"/>
+  </rcc>
+  <rcc rId="1156" sId="2">
+    <oc r="B56" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B56"/>
+  </rcc>
+  <rcc rId="1157" sId="2">
+    <oc r="B57" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B57"/>
+  </rcc>
+  <rcc rId="1158" sId="2">
+    <oc r="B58" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B58"/>
+  </rcc>
+  <rcc rId="1159" sId="2">
+    <oc r="B59" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B59"/>
+  </rcc>
+  <rcc rId="1160" sId="2">
+    <oc r="B60" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B60"/>
+  </rcc>
+  <rcc rId="1161" sId="2">
+    <oc r="B61" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B61"/>
+  </rcc>
+  <rcc rId="1162" sId="2">
+    <oc r="B62" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B62"/>
+  </rcc>
+  <rcc rId="1163" sId="2">
+    <oc r="B63" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B63"/>
+  </rcc>
+  <rcc rId="1164" sId="2">
+    <oc r="B64" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B64"/>
+  </rcc>
+  <rcc rId="1165" sId="2">
+    <oc r="B65" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B65"/>
+  </rcc>
+  <rcc rId="1166" sId="2">
+    <oc r="B66" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B66"/>
+  </rcc>
+  <rcc rId="1167" sId="2">
+    <oc r="B67" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B67"/>
+  </rcc>
+  <rcc rId="1168" sId="2">
+    <oc r="B68" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B68"/>
+  </rcc>
+  <rcc rId="1169" sId="2">
+    <oc r="B69" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B69"/>
+  </rcc>
+  <rcc rId="1170" sId="2">
+    <oc r="B70" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B70"/>
+  </rcc>
+  <rcc rId="1171" sId="2">
+    <oc r="B71" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B71"/>
+  </rcc>
+  <rcc rId="1172" sId="2">
+    <oc r="B72" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B72"/>
+  </rcc>
+  <rcc rId="1173" sId="2">
+    <oc r="B73" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B73"/>
+  </rcc>
+  <rcc rId="1174" sId="2">
+    <oc r="B74" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B74"/>
+  </rcc>
+  <rcc rId="1175" sId="2">
+    <oc r="B75" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B75"/>
+  </rcc>
+  <rcc rId="1176" sId="2">
+    <oc r="B76" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B76"/>
+  </rcc>
+  <rcc rId="1177" sId="2">
+    <oc r="B77" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B77"/>
+  </rcc>
+  <rcc rId="1178" sId="2">
+    <oc r="B78" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B78"/>
+  </rcc>
+  <rcc rId="1179" sId="2">
+    <oc r="B79" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B79"/>
+  </rcc>
+  <rcc rId="1180" sId="2">
+    <oc r="B80" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B80"/>
+  </rcc>
+  <rcc rId="1181" sId="2">
+    <oc r="B81" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B81"/>
+  </rcc>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="delete"/>
+  <rdn rId="0" localSheetId="2" customView="1" name="Z_E811CF45_D5B3_4449_84AE_1514F9E9258F_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>case!$A$2:$AD$2</formula>
+    <oldFormula>case!$A$2:$AD$2</oldFormula>
+  </rdn>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog17.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="delete"/>
+  <rdn rId="0" localSheetId="2" customView="1" name="Z_E811CF45_D5B3_4449_84AE_1514F9E9258F_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>case!$A$2:$AD$2</formula>
+    <oldFormula>case!$A$2:$AD$2</oldFormula>
+  </rdn>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog18.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="delete"/>
+  <rdn rId="0" localSheetId="2" customView="1" name="Z_E811CF45_D5B3_4449_84AE_1514F9E9258F_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>case!$A$2:$AD$2</formula>
+    <oldFormula>case!$A$2:$AD$2</oldFormula>
+  </rdn>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog19.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="delete"/>
   <rdn rId="0" localSheetId="2" customView="1" name="Z_E811CF45_D5B3_4449_84AE_1514F9E9258F_.wvu.FilterData" hidden="1" oldHidden="1">
     <formula>case!$A$2:$AD$2</formula>
@@ -13288,7 +14611,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -13373,8 +14698,8 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="BrxOpSv5Qn+u2wRjM+utC6UYLrvUI+Gay+w6zPQp8zz+/5I1udizjqbZ6brqgp9h1Ud3zJVEOn/q/bgrm9i81A==" saltValue="wt9VphKaQ5GnARCLMZGRjA==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <customSheetViews>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
-      <selection activeCell="B12" sqref="B12"/>
+    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
+      <selection activeCell="B35" sqref="B35"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -13383,8 +14708,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
-      <selection activeCell="B35" sqref="B35"/>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
@@ -13397,7 +14721,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD82"/>
+  <dimension ref="A1:AD83"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
@@ -14924,16 +16248,33 @@
         <v>429</v>
       </c>
     </row>
+    <row r="83" spans="1:19">
+      <c r="A83" s="18" t="s">
+        <v>434</v>
+      </c>
+      <c r="D83" s="18" t="s">
+        <v>371</v>
+      </c>
+      <c r="E83" s="18" t="s">
+        <v>435</v>
+      </c>
+      <c r="F83" s="18">
+        <v>2</v>
+      </c>
+      <c r="S83" s="18" t="s">
+        <v>429</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="4C55417S7/WEfM6p9p+2qxLa3pFuuwTQvkVS+xLflxPJ6JUMhmXb8UBi2EhWPKsWHpV7wPPZoM4Ci73L5pzjfA==" saltValue="OVPlytvnGy6tQU/SUgOtyg==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <autoFilter ref="A2:AD2"/>
   <customSheetViews>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" showAutoFilter="1">
+    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" scale="85" showAutoFilter="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-      <autoFilter ref="A2:AD2"/>
+      <autoFilter ref="A2:Y2"/>
     </customSheetView>
     <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" scale="85" showAutoFilter="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
@@ -14942,12 +16283,12 @@
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
       <autoFilter ref="A2:Y2"/>
     </customSheetView>
-    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" scale="85" showAutoFilter="1">
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" showAutoFilter="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
-      <autoFilter ref="A2:Y2"/>
+      <autoFilter ref="A2:AD2"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="2">
@@ -15088,17 +16429,17 @@
       <c r="E109" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="F109" s="93" t="s">
+      <c r="F109" s="73" t="s">
         <v>64</v>
       </c>
-      <c r="G109" s="94"/>
-      <c r="H109" s="94"/>
-      <c r="I109" s="94"/>
-      <c r="J109" s="94"/>
-      <c r="K109" s="94"/>
-      <c r="L109" s="94"/>
-      <c r="M109" s="94"/>
-      <c r="N109" s="95"/>
+      <c r="G109" s="74"/>
+      <c r="H109" s="74"/>
+      <c r="I109" s="74"/>
+      <c r="J109" s="74"/>
+      <c r="K109" s="74"/>
+      <c r="L109" s="74"/>
+      <c r="M109" s="74"/>
+      <c r="N109" s="75"/>
     </row>
     <row r="110" spans="1:14">
       <c r="A110" s="6" t="s">
@@ -15936,7 +17277,7 @@
       <c r="A144" s="41">
         <v>1</v>
       </c>
-      <c r="B144" s="96" t="s">
+      <c r="B144" s="76" t="s">
         <v>122</v>
       </c>
       <c r="C144" s="39" t="s">
@@ -15962,7 +17303,7 @@
       <c r="A145" s="41">
         <v>2</v>
       </c>
-      <c r="B145" s="97"/>
+      <c r="B145" s="77"/>
       <c r="C145" s="39" t="s">
         <v>128</v>
       </c>
@@ -15984,7 +17325,7 @@
       <c r="A146" s="59">
         <v>3</v>
       </c>
-      <c r="B146" s="97"/>
+      <c r="B146" s="77"/>
       <c r="C146" s="39" t="s">
         <v>9</v>
       </c>
@@ -16002,7 +17343,7 @@
       <c r="A147" s="59">
         <v>4</v>
       </c>
-      <c r="B147" s="97"/>
+      <c r="B147" s="77"/>
       <c r="C147" s="60" t="s">
         <v>256</v>
       </c>
@@ -16024,7 +17365,7 @@
       <c r="A148" s="59">
         <v>5</v>
       </c>
-      <c r="B148" s="97"/>
+      <c r="B148" s="77"/>
       <c r="C148" s="39" t="s">
         <v>253</v>
       </c>
@@ -16044,7 +17385,7 @@
       <c r="A149" s="59">
         <v>6</v>
       </c>
-      <c r="B149" s="97"/>
+      <c r="B149" s="77"/>
       <c r="C149" s="60" t="s">
         <v>254</v>
       </c>
@@ -16066,7 +17407,7 @@
       <c r="A150" s="59">
         <v>7</v>
       </c>
-      <c r="B150" s="97"/>
+      <c r="B150" s="77"/>
       <c r="C150" s="39" t="s">
         <v>130</v>
       </c>
@@ -16088,7 +17429,7 @@
       <c r="A151" s="59">
         <v>8</v>
       </c>
-      <c r="B151" s="97"/>
+      <c r="B151" s="77"/>
       <c r="C151" s="39" t="s">
         <v>246</v>
       </c>
@@ -16110,7 +17451,7 @@
       <c r="A152" s="59">
         <v>9</v>
       </c>
-      <c r="B152" s="97"/>
+      <c r="B152" s="77"/>
       <c r="C152" s="39" t="s">
         <v>55</v>
       </c>
@@ -16134,7 +17475,7 @@
       <c r="A153" s="59">
         <v>10</v>
       </c>
-      <c r="B153" s="83"/>
+      <c r="B153" s="78"/>
       <c r="C153" s="39" t="s">
         <v>136</v>
       </c>
@@ -16156,7 +17497,7 @@
       <c r="A154" s="59">
         <v>11</v>
       </c>
-      <c r="B154" s="79" t="s">
+      <c r="B154" s="72" t="s">
         <v>139</v>
       </c>
       <c r="C154" s="39" t="s">
@@ -16182,7 +17523,7 @@
       <c r="A155" s="59">
         <v>12</v>
       </c>
-      <c r="B155" s="79"/>
+      <c r="B155" s="72"/>
       <c r="C155" s="39" t="s">
         <v>247</v>
       </c>
@@ -16206,7 +17547,7 @@
       <c r="A156" s="59">
         <v>13</v>
       </c>
-      <c r="B156" s="96" t="s">
+      <c r="B156" s="76" t="s">
         <v>143</v>
       </c>
       <c r="C156" s="39" t="s">
@@ -16230,7 +17571,7 @@
       <c r="A157" s="59">
         <v>14</v>
       </c>
-      <c r="B157" s="83"/>
+      <c r="B157" s="78"/>
       <c r="C157" s="39" t="s">
         <v>146</v>
       </c>
@@ -16250,7 +17591,7 @@
       <c r="A158" s="59">
         <v>15</v>
       </c>
-      <c r="B158" s="79" t="s">
+      <c r="B158" s="72" t="s">
         <v>148</v>
       </c>
       <c r="C158" s="39" t="s">
@@ -16274,7 +17615,7 @@
       <c r="A159" s="59">
         <v>16</v>
       </c>
-      <c r="B159" s="79"/>
+      <c r="B159" s="72"/>
       <c r="C159" s="39" t="s">
         <v>152</v>
       </c>
@@ -16294,7 +17635,7 @@
       <c r="A160" s="59">
         <v>17</v>
       </c>
-      <c r="B160" s="79"/>
+      <c r="B160" s="72"/>
       <c r="C160" s="39" t="s">
         <v>153</v>
       </c>
@@ -16314,7 +17655,7 @@
       <c r="A161" s="59">
         <v>18</v>
       </c>
-      <c r="B161" s="79"/>
+      <c r="B161" s="72"/>
       <c r="C161" s="39" t="s">
         <v>154</v>
       </c>
@@ -16334,7 +17675,7 @@
       <c r="A162" s="59">
         <v>19</v>
       </c>
-      <c r="B162" s="79"/>
+      <c r="B162" s="72"/>
       <c r="C162" s="39" t="s">
         <v>155</v>
       </c>
@@ -16354,7 +17695,7 @@
       <c r="A163" s="59">
         <v>20</v>
       </c>
-      <c r="B163" s="79"/>
+      <c r="B163" s="72"/>
       <c r="C163" s="39" t="s">
         <v>156</v>
       </c>
@@ -16374,7 +17715,7 @@
       <c r="A164" s="59">
         <v>21</v>
       </c>
-      <c r="B164" s="79"/>
+      <c r="B164" s="72"/>
       <c r="C164" s="39" t="s">
         <v>157</v>
       </c>
@@ -16394,7 +17735,7 @@
       <c r="A165" s="59">
         <v>22</v>
       </c>
-      <c r="B165" s="79"/>
+      <c r="B165" s="72"/>
       <c r="C165" s="39" t="s">
         <v>158</v>
       </c>
@@ -16414,7 +17755,7 @@
       <c r="A166" s="59">
         <v>23</v>
       </c>
-      <c r="B166" s="79" t="s">
+      <c r="B166" s="72" t="s">
         <v>159</v>
       </c>
       <c r="C166" s="39" t="s">
@@ -16438,7 +17779,7 @@
       <c r="A167" s="59">
         <v>24</v>
       </c>
-      <c r="B167" s="79"/>
+      <c r="B167" s="72"/>
       <c r="C167" s="39" t="s">
         <v>163</v>
       </c>
@@ -16460,7 +17801,7 @@
       <c r="A168" s="59">
         <v>25</v>
       </c>
-      <c r="B168" s="79"/>
+      <c r="B168" s="72"/>
       <c r="C168" s="39" t="s">
         <v>166</v>
       </c>
@@ -16482,7 +17823,7 @@
       <c r="A169" s="59">
         <v>26</v>
       </c>
-      <c r="B169" s="79" t="s">
+      <c r="B169" s="72" t="s">
         <v>169</v>
       </c>
       <c r="C169" s="39" t="s">
@@ -16506,7 +17847,7 @@
       <c r="A170" s="59">
         <v>27</v>
       </c>
-      <c r="B170" s="79"/>
+      <c r="B170" s="72"/>
       <c r="C170" s="39" t="s">
         <v>172</v>
       </c>
@@ -16528,7 +17869,7 @@
       <c r="A171" s="42">
         <v>28</v>
       </c>
-      <c r="B171" s="80"/>
+      <c r="B171" s="79"/>
       <c r="C171" s="40"/>
       <c r="D171" s="40"/>
       <c r="E171" s="40"/>
@@ -16564,11 +17905,11 @@
       <c r="B185" s="26" t="s">
         <v>178</v>
       </c>
-      <c r="C185" s="89" t="s">
+      <c r="C185" s="80" t="s">
         <v>43</v>
       </c>
-      <c r="D185" s="89"/>
-      <c r="E185" s="89"/>
+      <c r="D185" s="80"/>
+      <c r="E185" s="80"/>
       <c r="F185" s="34" t="s">
         <v>42</v>
       </c>
@@ -16577,17 +17918,17 @@
       </c>
     </row>
     <row r="186" spans="1:7">
-      <c r="A186" s="79" t="s">
+      <c r="A186" s="72" t="s">
         <v>180</v>
       </c>
-      <c r="B186" s="79" t="s">
+      <c r="B186" s="72" t="s">
         <v>181</v>
       </c>
-      <c r="C186" s="90" t="s">
+      <c r="C186" s="81" t="s">
         <v>182</v>
       </c>
-      <c r="D186" s="90"/>
-      <c r="E186" s="90"/>
+      <c r="D186" s="81"/>
+      <c r="E186" s="81"/>
       <c r="F186" s="39" t="s">
         <v>183</v>
       </c>
@@ -16596,13 +17937,13 @@
       </c>
     </row>
     <row r="187" spans="1:7">
-      <c r="A187" s="79"/>
-      <c r="B187" s="79"/>
-      <c r="C187" s="91" t="s">
+      <c r="A187" s="72"/>
+      <c r="B187" s="72"/>
+      <c r="C187" s="82" t="s">
         <v>56</v>
       </c>
-      <c r="D187" s="91"/>
-      <c r="E187" s="91"/>
+      <c r="D187" s="82"/>
+      <c r="E187" s="82"/>
       <c r="F187" s="39" t="s">
         <v>185</v>
       </c>
@@ -16611,15 +17952,15 @@
       </c>
     </row>
     <row r="188" spans="1:7">
-      <c r="A188" s="79"/>
-      <c r="B188" s="79" t="s">
+      <c r="A188" s="72"/>
+      <c r="B188" s="72" t="s">
         <v>186</v>
       </c>
-      <c r="C188" s="92" t="s">
+      <c r="C188" s="83" t="s">
         <v>187</v>
       </c>
-      <c r="D188" s="92"/>
-      <c r="E188" s="92"/>
+      <c r="D188" s="83"/>
+      <c r="E188" s="83"/>
       <c r="F188" s="39" t="s">
         <v>183</v>
       </c>
@@ -16628,13 +17969,13 @@
       </c>
     </row>
     <row r="189" spans="1:7">
-      <c r="A189" s="79"/>
-      <c r="B189" s="79"/>
-      <c r="C189" s="92" t="s">
+      <c r="A189" s="72"/>
+      <c r="B189" s="72"/>
+      <c r="C189" s="83" t="s">
         <v>187</v>
       </c>
-      <c r="D189" s="92"/>
-      <c r="E189" s="92"/>
+      <c r="D189" s="83"/>
+      <c r="E189" s="83"/>
       <c r="F189" s="39" t="s">
         <v>185</v>
       </c>
@@ -16643,17 +17984,17 @@
       </c>
     </row>
     <row r="190" spans="1:7">
-      <c r="A190" s="77" t="s">
+      <c r="A190" s="84" t="s">
         <v>188</v>
       </c>
-      <c r="B190" s="79" t="s">
+      <c r="B190" s="72" t="s">
         <v>189</v>
       </c>
-      <c r="C190" s="79" t="s">
+      <c r="C190" s="72" t="s">
         <v>44</v>
       </c>
-      <c r="D190" s="79"/>
-      <c r="E190" s="79"/>
+      <c r="D190" s="72"/>
+      <c r="E190" s="72"/>
       <c r="F190" s="39" t="s">
         <v>183</v>
       </c>
@@ -16662,13 +18003,13 @@
       </c>
     </row>
     <row r="191" spans="1:7">
-      <c r="A191" s="77"/>
-      <c r="B191" s="79"/>
-      <c r="C191" s="79" t="s">
+      <c r="A191" s="84"/>
+      <c r="B191" s="72"/>
+      <c r="C191" s="72" t="s">
         <v>45</v>
       </c>
-      <c r="D191" s="79"/>
-      <c r="E191" s="79"/>
+      <c r="D191" s="72"/>
+      <c r="E191" s="72"/>
       <c r="F191" s="39" t="s">
         <v>185</v>
       </c>
@@ -16677,15 +18018,15 @@
       </c>
     </row>
     <row r="192" spans="1:7">
-      <c r="A192" s="77"/>
-      <c r="B192" s="79" t="s">
+      <c r="A192" s="84"/>
+      <c r="B192" s="72" t="s">
         <v>190</v>
       </c>
-      <c r="C192" s="79" t="s">
+      <c r="C192" s="72" t="s">
         <v>46</v>
       </c>
-      <c r="D192" s="79"/>
-      <c r="E192" s="79"/>
+      <c r="D192" s="72"/>
+      <c r="E192" s="72"/>
       <c r="F192" s="39" t="s">
         <v>183</v>
       </c>
@@ -16694,13 +18035,13 @@
       </c>
     </row>
     <row r="193" spans="1:7">
-      <c r="A193" s="77"/>
-      <c r="B193" s="79"/>
-      <c r="C193" s="79" t="s">
+      <c r="A193" s="84"/>
+      <c r="B193" s="72"/>
+      <c r="C193" s="72" t="s">
         <v>47</v>
       </c>
-      <c r="D193" s="79"/>
-      <c r="E193" s="79"/>
+      <c r="D193" s="72"/>
+      <c r="E193" s="72"/>
       <c r="F193" s="39" t="s">
         <v>185</v>
       </c>
@@ -16709,17 +18050,17 @@
       </c>
     </row>
     <row r="194" spans="1:7">
-      <c r="A194" s="77" t="s">
+      <c r="A194" s="84" t="s">
         <v>191</v>
       </c>
-      <c r="B194" s="79" t="s">
+      <c r="B194" s="72" t="s">
         <v>192</v>
       </c>
-      <c r="C194" s="79" t="s">
+      <c r="C194" s="72" t="s">
         <v>48</v>
       </c>
-      <c r="D194" s="79"/>
-      <c r="E194" s="79"/>
+      <c r="D194" s="72"/>
+      <c r="E194" s="72"/>
       <c r="F194" s="39" t="s">
         <v>183</v>
       </c>
@@ -16728,13 +18069,13 @@
       </c>
     </row>
     <row r="195" spans="1:7">
-      <c r="A195" s="77"/>
-      <c r="B195" s="79"/>
-      <c r="C195" s="79" t="s">
+      <c r="A195" s="84"/>
+      <c r="B195" s="72"/>
+      <c r="C195" s="72" t="s">
         <v>49</v>
       </c>
-      <c r="D195" s="79"/>
-      <c r="E195" s="79"/>
+      <c r="D195" s="72"/>
+      <c r="E195" s="72"/>
       <c r="F195" s="39" t="s">
         <v>185</v>
       </c>
@@ -16743,15 +18084,15 @@
       </c>
     </row>
     <row r="196" spans="1:7">
-      <c r="A196" s="77"/>
-      <c r="B196" s="79" t="s">
+      <c r="A196" s="84"/>
+      <c r="B196" s="72" t="s">
         <v>193</v>
       </c>
-      <c r="C196" s="79" t="s">
+      <c r="C196" s="72" t="s">
         <v>194</v>
       </c>
-      <c r="D196" s="79"/>
-      <c r="E196" s="79"/>
+      <c r="D196" s="72"/>
+      <c r="E196" s="72"/>
       <c r="F196" s="39" t="s">
         <v>183</v>
       </c>
@@ -16760,13 +18101,13 @@
       </c>
     </row>
     <row r="197" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A197" s="78"/>
-      <c r="B197" s="80"/>
-      <c r="C197" s="80" t="s">
+      <c r="A197" s="86"/>
+      <c r="B197" s="79"/>
+      <c r="C197" s="79" t="s">
         <v>195</v>
       </c>
-      <c r="D197" s="80"/>
-      <c r="E197" s="80"/>
+      <c r="D197" s="79"/>
+      <c r="E197" s="79"/>
       <c r="F197" s="40" t="s">
         <v>185</v>
       </c>
@@ -16805,12 +18146,12 @@
       <c r="A202" s="21" t="s">
         <v>197</v>
       </c>
-      <c r="B202" s="81" t="s">
+      <c r="B202" s="87" t="s">
         <v>198</v>
       </c>
-      <c r="C202" s="81"/>
-      <c r="D202" s="81"/>
-      <c r="E202" s="81"/>
+      <c r="C202" s="87"/>
+      <c r="D202" s="87"/>
+      <c r="E202" s="87"/>
       <c r="F202" s="22" t="s">
         <v>199</v>
       </c>
@@ -16822,12 +18163,12 @@
       <c r="A203" s="35" t="s">
         <v>201</v>
       </c>
-      <c r="B203" s="82" t="s">
+      <c r="B203" s="88" t="s">
         <v>202</v>
       </c>
-      <c r="C203" s="83"/>
-      <c r="D203" s="83"/>
-      <c r="E203" s="83"/>
+      <c r="C203" s="78"/>
+      <c r="D203" s="78"/>
+      <c r="E203" s="78"/>
       <c r="F203" s="36" t="s">
         <v>203</v>
       </c>
@@ -16839,12 +18180,12 @@
       <c r="A204" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="B204" s="84" t="s">
+      <c r="B204" s="89" t="s">
         <v>205</v>
       </c>
-      <c r="C204" s="85"/>
-      <c r="D204" s="85"/>
-      <c r="E204" s="86"/>
+      <c r="C204" s="90"/>
+      <c r="D204" s="90"/>
+      <c r="E204" s="91"/>
       <c r="F204" s="10" t="s">
         <v>184</v>
       </c>
@@ -16856,12 +18197,12 @@
       <c r="A205" s="45" t="s">
         <v>230</v>
       </c>
-      <c r="B205" s="84" t="s">
+      <c r="B205" s="89" t="s">
         <v>233</v>
       </c>
-      <c r="C205" s="85"/>
-      <c r="D205" s="85"/>
-      <c r="E205" s="86"/>
+      <c r="C205" s="90"/>
+      <c r="D205" s="90"/>
+      <c r="E205" s="91"/>
       <c r="F205" s="46" t="s">
         <v>231</v>
       </c>
@@ -16873,12 +18214,12 @@
       <c r="A206" s="12" t="s">
         <v>232</v>
       </c>
-      <c r="B206" s="87" t="s">
+      <c r="B206" s="92" t="s">
         <v>234</v>
       </c>
-      <c r="C206" s="80"/>
-      <c r="D206" s="80"/>
-      <c r="E206" s="80"/>
+      <c r="C206" s="79"/>
+      <c r="D206" s="79"/>
+      <c r="E206" s="79"/>
       <c r="F206" s="13" t="s">
         <v>184</v>
       </c>
@@ -16923,11 +18264,11 @@
       <c r="C211" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="D211" s="88" t="s">
+      <c r="D211" s="93" t="s">
         <v>53</v>
       </c>
-      <c r="E211" s="88"/>
-      <c r="F211" s="88"/>
+      <c r="E211" s="93"/>
+      <c r="F211" s="93"/>
       <c r="G211" s="32"/>
     </row>
     <row r="212" spans="1:7">
@@ -16940,11 +18281,11 @@
       <c r="C212" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="D212" s="72" t="s">
+      <c r="D212" s="85" t="s">
         <v>54</v>
       </c>
-      <c r="E212" s="72"/>
-      <c r="F212" s="72"/>
+      <c r="E212" s="85"/>
+      <c r="F212" s="85"/>
       <c r="G212" s="24"/>
     </row>
     <row r="213" spans="1:7">
@@ -16957,11 +18298,11 @@
       <c r="C213" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="D213" s="72" t="s">
+      <c r="D213" s="85" t="s">
         <v>209</v>
       </c>
-      <c r="E213" s="72"/>
-      <c r="F213" s="72"/>
+      <c r="E213" s="85"/>
+      <c r="F213" s="85"/>
       <c r="G213" s="24"/>
     </row>
     <row r="214" spans="1:7">
@@ -16974,11 +18315,11 @@
       <c r="C214" s="39" t="s">
         <v>210</v>
       </c>
-      <c r="D214" s="72" t="s">
+      <c r="D214" s="85" t="s">
         <v>211</v>
       </c>
-      <c r="E214" s="72"/>
-      <c r="F214" s="72"/>
+      <c r="E214" s="85"/>
+      <c r="F214" s="85"/>
       <c r="G214" s="24"/>
     </row>
     <row r="215" spans="1:7">
@@ -16991,11 +18332,11 @@
       <c r="C215" s="44" t="s">
         <v>210</v>
       </c>
-      <c r="D215" s="72" t="s">
+      <c r="D215" s="85" t="s">
         <v>222</v>
       </c>
-      <c r="E215" s="72"/>
-      <c r="F215" s="72"/>
+      <c r="E215" s="85"/>
+      <c r="F215" s="85"/>
       <c r="G215" s="24"/>
     </row>
     <row r="216" spans="1:7">
@@ -17008,11 +18349,11 @@
       <c r="C216" s="39" t="s">
         <v>236</v>
       </c>
-      <c r="D216" s="72" t="s">
+      <c r="D216" s="85" t="s">
         <v>235</v>
       </c>
-      <c r="E216" s="72"/>
-      <c r="F216" s="72"/>
+      <c r="E216" s="85"/>
+      <c r="F216" s="85"/>
       <c r="G216" s="24"/>
     </row>
     <row r="217" spans="1:7">
@@ -17025,11 +18366,11 @@
       <c r="C217" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="D217" s="74" t="s">
+      <c r="D217" s="95" t="s">
         <v>237</v>
       </c>
-      <c r="E217" s="75"/>
-      <c r="F217" s="76"/>
+      <c r="E217" s="96"/>
+      <c r="F217" s="97"/>
       <c r="G217" s="53"/>
     </row>
     <row r="218" spans="1:7">
@@ -17042,11 +18383,11 @@
       <c r="C218" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="D218" s="74" t="s">
+      <c r="D218" s="95" t="s">
         <v>238</v>
       </c>
-      <c r="E218" s="75"/>
-      <c r="F218" s="76"/>
+      <c r="E218" s="96"/>
+      <c r="F218" s="97"/>
       <c r="G218" s="53"/>
     </row>
     <row r="219" spans="1:7">
@@ -17059,11 +18400,11 @@
       <c r="C219" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="D219" s="74" t="s">
+      <c r="D219" s="95" t="s">
         <v>251</v>
       </c>
-      <c r="E219" s="75"/>
-      <c r="F219" s="76"/>
+      <c r="E219" s="96"/>
+      <c r="F219" s="97"/>
       <c r="G219" s="53"/>
     </row>
     <row r="220" spans="1:7">
@@ -17110,11 +18451,11 @@
       <c r="C222" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="D222" s="73" t="s">
+      <c r="D222" s="94" t="s">
         <v>264</v>
       </c>
-      <c r="E222" s="73"/>
-      <c r="F222" s="73"/>
+      <c r="E222" s="94"/>
+      <c r="F222" s="94"/>
       <c r="G222" s="25"/>
     </row>
   </sheetData>
@@ -17127,28 +18468,14 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="44">
-    <mergeCell ref="B166:B168"/>
-    <mergeCell ref="F109:N109"/>
-    <mergeCell ref="B144:B153"/>
-    <mergeCell ref="B154:B155"/>
-    <mergeCell ref="B156:B157"/>
-    <mergeCell ref="B158:B165"/>
-    <mergeCell ref="B169:B171"/>
-    <mergeCell ref="C185:E185"/>
-    <mergeCell ref="A186:A189"/>
-    <mergeCell ref="B186:B187"/>
-    <mergeCell ref="C186:E186"/>
-    <mergeCell ref="C187:E187"/>
-    <mergeCell ref="B188:B189"/>
-    <mergeCell ref="C188:E188"/>
-    <mergeCell ref="C189:E189"/>
-    <mergeCell ref="A190:A193"/>
-    <mergeCell ref="B190:B191"/>
-    <mergeCell ref="C190:E190"/>
-    <mergeCell ref="C191:E191"/>
-    <mergeCell ref="B192:B193"/>
-    <mergeCell ref="C192:E192"/>
-    <mergeCell ref="C193:E193"/>
+    <mergeCell ref="D213:F213"/>
+    <mergeCell ref="D214:F214"/>
+    <mergeCell ref="D215:F215"/>
+    <mergeCell ref="D216:F216"/>
+    <mergeCell ref="D222:F222"/>
+    <mergeCell ref="D217:F217"/>
+    <mergeCell ref="D218:F218"/>
+    <mergeCell ref="D219:F219"/>
     <mergeCell ref="D212:F212"/>
     <mergeCell ref="A194:A197"/>
     <mergeCell ref="B194:B195"/>
@@ -17163,14 +18490,28 @@
     <mergeCell ref="B206:E206"/>
     <mergeCell ref="D211:F211"/>
     <mergeCell ref="B205:E205"/>
-    <mergeCell ref="D213:F213"/>
-    <mergeCell ref="D214:F214"/>
-    <mergeCell ref="D215:F215"/>
-    <mergeCell ref="D216:F216"/>
-    <mergeCell ref="D222:F222"/>
-    <mergeCell ref="D217:F217"/>
-    <mergeCell ref="D218:F218"/>
-    <mergeCell ref="D219:F219"/>
+    <mergeCell ref="A190:A193"/>
+    <mergeCell ref="B190:B191"/>
+    <mergeCell ref="C190:E190"/>
+    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="B192:B193"/>
+    <mergeCell ref="C192:E192"/>
+    <mergeCell ref="C193:E193"/>
+    <mergeCell ref="B169:B171"/>
+    <mergeCell ref="C185:E185"/>
+    <mergeCell ref="A186:A189"/>
+    <mergeCell ref="B186:B187"/>
+    <mergeCell ref="C186:E186"/>
+    <mergeCell ref="C187:E187"/>
+    <mergeCell ref="B188:B189"/>
+    <mergeCell ref="C188:E188"/>
+    <mergeCell ref="C189:E189"/>
+    <mergeCell ref="B166:B168"/>
+    <mergeCell ref="F109:N109"/>
+    <mergeCell ref="B144:B153"/>
+    <mergeCell ref="B154:B155"/>
+    <mergeCell ref="B156:B157"/>
+    <mergeCell ref="B158:B165"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17194,15 +18535,15 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
+      <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
       <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
-      <selection activeCell="E26" sqref="E26"/>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>